<commit_message>
add DT line 2 mrt stations
</commit_message>
<xml_diff>
--- a/inputdata/MRT.xlsx
+++ b/inputdata/MRT.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiangnanqing/Dropbox/project/busstoppy/inputdata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27792" windowHeight="12576"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="588">
   <si>
     <t>Number</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -634,10 +644,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>？兰站</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>30 Woodlands Avenue 2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2272,6 +2278,81 @@
   <si>
     <t>60 Sengkang E Ave</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DT13</t>
+  </si>
+  <si>
+    <t>DT12</t>
+  </si>
+  <si>
+    <t>DT1</t>
+  </si>
+  <si>
+    <t>DT2</t>
+  </si>
+  <si>
+    <t>DT3</t>
+  </si>
+  <si>
+    <t>DT5</t>
+  </si>
+  <si>
+    <t>DT6</t>
+  </si>
+  <si>
+    <t>DT7</t>
+  </si>
+  <si>
+    <t>DT8</t>
+  </si>
+  <si>
+    <t>DT9</t>
+  </si>
+  <si>
+    <t>DT10</t>
+  </si>
+  <si>
+    <t>DT11</t>
+  </si>
+  <si>
+    <t>Bukit Panjang</t>
+  </si>
+  <si>
+    <t>Cashew</t>
+  </si>
+  <si>
+    <t>Hillview</t>
+  </si>
+  <si>
+    <t>Beauty World</t>
+  </si>
+  <si>
+    <t>King Albert Park</t>
+  </si>
+  <si>
+    <t>Sixth Avenue</t>
+  </si>
+  <si>
+    <t>Tan Kah Kee</t>
+  </si>
+  <si>
+    <t>Botanic Gardens</t>
+  </si>
+  <si>
+    <t>Stevens</t>
+  </si>
+  <si>
+    <t>Newton</t>
+  </si>
+  <si>
+    <t>Little India</t>
+  </si>
+  <si>
+    <t>Rochor</t>
+  </si>
+  <si>
+    <t>兀兰站</t>
   </si>
 </sst>
 </file>
@@ -2281,7 +2362,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000_ "/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2348,7 +2429,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2396,6 +2477,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2454,12 +2538,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -2489,12 +2573,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -2698,24 +2782,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H143"/>
+  <dimension ref="A1:H155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="2" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
     <col min="7" max="7" width="30.6640625" customWidth="1"/>
-    <col min="8" max="8" width="25.77734375" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2741,7 +2826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2764,7 +2849,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2787,7 +2872,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2807,7 +2892,7 @@
         <v>649846</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2830,7 +2915,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -2853,7 +2938,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -2876,7 +2961,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2899,7 +2984,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2920,7 +3005,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2943,7 +3028,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -2966,7 +3051,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -2987,7 +3072,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -3010,7 +3095,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>55</v>
       </c>
@@ -3033,7 +3118,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -3056,7 +3141,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -3076,7 +3161,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -3099,7 +3184,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>72</v>
       </c>
@@ -3122,7 +3207,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -3145,7 +3230,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>79</v>
       </c>
@@ -3162,7 +3247,7 @@
         <v>103.86299099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -3179,7 +3264,7 @@
         <v>103.871392</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -3196,7 +3281,7 @@
         <v>103.882893</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -3216,7 +3301,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -3239,7 +3324,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -3262,7 +3347,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -3279,7 +3364,7 @@
         <v>103.930025</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -3302,7 +3387,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -3322,7 +3407,7 @@
         <v>489480</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -3342,7 +3427,7 @@
         <v>529538</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>115</v>
       </c>
@@ -3359,7 +3444,7 @@
         <v>103.949504</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>118</v>
       </c>
@@ -3379,7 +3464,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>122</v>
       </c>
@@ -3399,7 +3484,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -3419,7 +3504,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -3439,7 +3524,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>134</v>
       </c>
@@ -3462,7 +3547,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -3485,7 +3570,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -3508,7 +3593,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>146</v>
       </c>
@@ -3525,7 +3610,7 @@
         <v>103.76190099999999</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>149</v>
       </c>
@@ -3545,15 +3630,15 @@
         <v>739044</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
       <c r="B40" t="s">
         <v>153</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>154</v>
+      <c r="C40" s="16" t="s">
+        <v>587</v>
       </c>
       <c r="D40">
         <v>1.4371970000000001</v>
@@ -3565,18 +3650,18 @@
         <v>738343</v>
       </c>
       <c r="G40" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
         <v>156</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" s="10" t="s">
         <v>157</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>158</v>
       </c>
       <c r="D41">
         <v>1.440715</v>
@@ -3588,18 +3673,18 @@
         <v>738344</v>
       </c>
       <c r="G41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>160</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" s="10" t="s">
         <v>161</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>162</v>
       </c>
       <c r="D42">
         <v>1.4490810000000001</v>
@@ -3611,18 +3696,18 @@
         <v>759775</v>
       </c>
       <c r="G42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
         <v>164</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" s="10" t="s">
         <v>165</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>166</v>
       </c>
       <c r="D43">
         <v>1.4295610000000001</v>
@@ -3631,32 +3716,32 @@
         <v>103.83524300000001</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" t="s">
         <v>167</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" s="10" t="s">
         <v>168</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>169</v>
       </c>
       <c r="D44">
         <v>1.417548</v>
       </c>
       <c r="E44" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
         <v>171</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" s="10" t="s">
         <v>172</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>173</v>
       </c>
       <c r="D45">
         <v>1.3820790000000001</v>
@@ -3668,18 +3753,18 @@
         <v>569813</v>
       </c>
       <c r="G45" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
         <v>175</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" s="10" t="s">
         <v>176</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>177</v>
       </c>
       <c r="D46">
         <v>1.3700349999999999</v>
@@ -3691,18 +3776,18 @@
         <v>569811</v>
       </c>
       <c r="G46" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
         <v>179</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" s="10" t="s">
         <v>180</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>181</v>
       </c>
       <c r="D47">
         <v>1.350803</v>
@@ -3714,18 +3799,18 @@
         <v>579827</v>
       </c>
       <c r="G47" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
         <v>183</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" s="10" t="s">
         <v>184</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>185</v>
       </c>
       <c r="D48">
         <v>1.340292</v>
@@ -3737,18 +3822,18 @@
         <v>319758</v>
       </c>
       <c r="G48" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" t="s">
+      <c r="B49" t="s">
         <v>187</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" s="10" t="s">
         <v>188</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>189</v>
       </c>
       <c r="D49">
         <v>1.3327260000000001</v>
@@ -3760,18 +3845,18 @@
         <v>310190</v>
       </c>
       <c r="G49" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
         <v>191</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>193</v>
       </c>
       <c r="D50">
         <v>1.320038</v>
@@ -3783,18 +3868,18 @@
         <v>307683</v>
       </c>
       <c r="G50" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
         <v>195</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" s="10" t="s">
         <v>196</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>197</v>
       </c>
       <c r="D51">
         <v>1.312487</v>
@@ -3806,18 +3891,18 @@
         <v>228234</v>
       </c>
       <c r="G51" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" t="s">
+      <c r="B52" t="s">
         <v>199</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" s="10" t="s">
         <v>200</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>201</v>
       </c>
       <c r="D52">
         <v>1.304324</v>
@@ -3829,15 +3914,15 @@
         <v>238801</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>201</v>
+      </c>
+      <c r="B53" t="s">
         <v>202</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" s="10" t="s">
         <v>203</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>204</v>
       </c>
       <c r="D53">
         <v>1.300125</v>
@@ -3849,18 +3934,18 @@
         <v>238162</v>
       </c>
       <c r="G53" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" t="s">
+      <c r="B54" t="s">
         <v>206</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" s="10" t="s">
         <v>207</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>208</v>
       </c>
       <c r="D54">
         <v>1.2985910000000001</v>
@@ -3872,18 +3957,18 @@
         <v>238826</v>
       </c>
       <c r="G54" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" t="s">
+      <c r="B55" t="s">
         <v>210</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" s="10" t="s">
         <v>211</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>212</v>
       </c>
       <c r="D55">
         <v>1.293239</v>
@@ -3895,18 +3980,18 @@
         <v>179100</v>
       </c>
       <c r="G55" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" t="s">
+      <c r="B56" t="s">
         <v>214</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" s="10" t="s">
         <v>215</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>216</v>
       </c>
       <c r="D56">
         <v>1.2839389999999999</v>
@@ -3915,64 +4000,64 @@
         <v>103.851642</v>
       </c>
       <c r="F56" s="13" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" t="s">
+      <c r="B57" t="s">
         <v>218</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="C57" s="10" t="s">
-        <v>220</v>
-      </c>
       <c r="D57" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E57" s="7">
         <v>103.85480699999999</v>
       </c>
       <c r="F57" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="G57" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="G57" s="7" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>223</v>
+      </c>
+      <c r="B58" t="s">
         <v>224</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" s="10" t="s">
         <v>225</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>226</v>
       </c>
       <c r="D58">
         <v>1.2709710000000001</v>
       </c>
       <c r="E58" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>229</v>
       </c>
-      <c r="F58" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" t="s">
+      <c r="B59" t="s">
         <v>230</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" s="10" t="s">
         <v>231</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>232</v>
       </c>
       <c r="D59">
         <v>1.2652969999999999</v>
@@ -3981,21 +4066,21 @@
         <v>103.82118199999999</v>
       </c>
       <c r="F59" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="G59" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="G59" s="7" t="s">
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" t="s">
+      <c r="B60" t="s">
         <v>235</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" s="10" t="s">
         <v>236</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>237</v>
       </c>
       <c r="D60">
         <v>1.281344</v>
@@ -4004,15 +4089,15 @@
         <v>103.839765</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>237</v>
+      </c>
+      <c r="B61" t="s">
         <v>238</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" s="10" t="s">
         <v>239</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>240</v>
       </c>
       <c r="D61">
         <v>1.284446</v>
@@ -4022,18 +4107,18 @@
       </c>
       <c r="F61" s="13"/>
       <c r="G61" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>261</v>
+      </c>
+      <c r="B62" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" t="s">
-        <v>262</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="C62" s="10" t="s">
         <v>242</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>243</v>
       </c>
       <c r="D62">
         <v>1.2885009999999999</v>
@@ -4042,18 +4127,18 @@
         <v>103.846778</v>
       </c>
       <c r="G62" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B63" t="s">
+        <v>206</v>
+      </c>
+      <c r="C63" s="10" t="s">
         <v>207</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>208</v>
       </c>
       <c r="D63">
         <v>1.298594</v>
@@ -4065,18 +4150,18 @@
         <v>238826</v>
       </c>
       <c r="G63" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B64" t="s">
+        <v>244</v>
+      </c>
+      <c r="C64" s="10" t="s">
         <v>245</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>246</v>
       </c>
       <c r="D64" s="10">
         <v>1.3072280000000001</v>
@@ -4085,38 +4170,38 @@
         <v>103.849847</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B65" t="s">
+        <v>246</v>
+      </c>
+      <c r="C65" s="10" t="s">
         <v>247</v>
-      </c>
-      <c r="C65" s="10" t="s">
-        <v>248</v>
       </c>
       <c r="D65" s="10">
         <v>1.3124089999999999</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F65">
         <v>217562</v>
       </c>
       <c r="G65" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B66" t="s">
+        <v>250</v>
+      </c>
+      <c r="C66" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="C66" s="10" t="s">
-        <v>252</v>
       </c>
       <c r="D66" s="10">
         <v>1.319596</v>
@@ -4128,15 +4213,15 @@
         <v>328260</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B67" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D67" s="10">
         <v>1.3313619999999999</v>
@@ -4148,18 +4233,18 @@
         <v>347663</v>
       </c>
       <c r="G67" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B68" t="s">
+        <v>255</v>
+      </c>
+      <c r="C68" s="10" t="s">
         <v>256</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>257</v>
       </c>
       <c r="D68" s="10">
         <v>1.3393630000000001</v>
@@ -4168,18 +4253,18 @@
         <v>103.870757</v>
       </c>
       <c r="G68" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>268</v>
+      </c>
+      <c r="B69" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" t="s">
-        <v>269</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="C69" s="10" t="s">
         <v>259</v>
-      </c>
-      <c r="C69" s="10" t="s">
-        <v>260</v>
       </c>
       <c r="D69" s="10">
         <v>1.3492420000000001</v>
@@ -4191,18 +4276,18 @@
         <v>534801</v>
       </c>
       <c r="G69" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>269</v>
+      </c>
+      <c r="B70" t="s">
         <v>270</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" s="10" t="s">
         <v>271</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>272</v>
       </c>
       <c r="D70" s="10">
         <v>1.3605149999999999</v>
@@ -4211,18 +4296,18 @@
         <v>103.885209</v>
       </c>
       <c r="G70" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" t="s">
+      <c r="B71" t="s">
         <v>274</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" s="10" t="s">
         <v>275</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>276</v>
       </c>
       <c r="D71" s="10">
         <v>1.370919</v>
@@ -4234,18 +4319,18 @@
         <v>538757</v>
       </c>
       <c r="G71" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" t="s">
+      <c r="B72" t="s">
         <v>278</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" s="10" t="s">
         <v>279</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>280</v>
       </c>
       <c r="D72" s="10">
         <v>1.382449</v>
@@ -4257,15 +4342,15 @@
         <v>549927</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>280</v>
+      </c>
+      <c r="B73" t="s">
+        <v>282</v>
+      </c>
+      <c r="C73" s="10" t="s">
         <v>281</v>
-      </c>
-      <c r="B73" t="s">
-        <v>283</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>282</v>
       </c>
       <c r="D73" s="10">
         <v>1.3912659999999999</v>
@@ -4277,18 +4362,18 @@
         <v>545062</v>
       </c>
       <c r="G73" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="A74" t="s">
+      <c r="B74" t="s">
         <v>285</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" s="10" t="s">
         <v>286</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>287</v>
       </c>
       <c r="D74" s="10">
         <v>1.4045449999999999</v>
@@ -4300,18 +4385,18 @@
         <v>828868</v>
       </c>
       <c r="G74" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" t="s">
-        <v>289</v>
-      </c>
       <c r="B75" t="s">
+        <v>206</v>
+      </c>
+      <c r="C75" s="10" t="s">
         <v>207</v>
-      </c>
-      <c r="C75" s="10" t="s">
-        <v>208</v>
       </c>
       <c r="D75" s="10">
         <v>1.298746</v>
@@ -4320,15 +4405,15 @@
         <v>103.844688</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>289</v>
+      </c>
+      <c r="B76" t="s">
         <v>290</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" s="10" t="s">
         <v>291</v>
-      </c>
-      <c r="C76" s="10" t="s">
-        <v>292</v>
       </c>
       <c r="D76" s="10">
         <v>1.2969440000000001</v>
@@ -4340,18 +4425,18 @@
         <v>189561</v>
       </c>
       <c r="G76" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" t="s">
+      <c r="B77" t="s">
         <v>294</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" s="10" t="s">
         <v>295</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>296</v>
       </c>
       <c r="D77" s="10">
         <v>1.2934680000000001</v>
@@ -4360,21 +4445,21 @@
         <v>103.855352</v>
       </c>
       <c r="F77" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="G77" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="G77" s="7" t="s">
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" t="s">
+      <c r="B78" t="s">
         <v>299</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" s="10" t="s">
         <v>300</v>
-      </c>
-      <c r="C78" s="10" t="s">
-        <v>301</v>
       </c>
       <c r="D78" s="10">
         <v>1.293147</v>
@@ -4383,21 +4468,21 @@
         <v>103.86082399999999</v>
       </c>
       <c r="F78" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>303</v>
       </c>
-      <c r="G78" s="7" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" t="s">
+      <c r="B79" t="s">
         <v>304</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" s="10" t="s">
         <v>305</v>
-      </c>
-      <c r="C79" s="10" t="s">
-        <v>306</v>
       </c>
       <c r="D79" s="10">
         <v>1.2997540000000001</v>
@@ -4406,21 +4491,21 @@
         <v>103.863699</v>
       </c>
       <c r="F79" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="G79" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="G79" s="7" t="s">
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" t="s">
+      <c r="B80" t="s">
         <v>309</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" s="10" t="s">
         <v>310</v>
-      </c>
-      <c r="C80" s="10" t="s">
-        <v>311</v>
       </c>
       <c r="D80" s="10">
         <v>1.302929</v>
@@ -4432,18 +4517,18 @@
         <v>397692</v>
       </c>
       <c r="G80" s="7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="A81" t="s">
+      <c r="B81" t="s">
         <v>313</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" s="10" t="s">
         <v>314</v>
-      </c>
-      <c r="C81" s="10" t="s">
-        <v>315</v>
       </c>
       <c r="D81" s="10">
         <v>1.3064039999999999</v>
@@ -4452,18 +4537,18 @@
         <v>103.882582</v>
       </c>
       <c r="G81" s="7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="82" spans="1:7">
-      <c r="A82" t="s">
+      <c r="B82" t="s">
         <v>317</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" s="10" t="s">
         <v>318</v>
-      </c>
-      <c r="C82" s="10" t="s">
-        <v>319</v>
       </c>
       <c r="D82" s="10">
         <v>1.308292</v>
@@ -4472,18 +4557,18 @@
         <v>103.88824700000001</v>
       </c>
       <c r="G82" s="7" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="83" spans="1:7">
-      <c r="A83" t="s">
+      <c r="B83" t="s">
         <v>321</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" s="10" t="s">
         <v>322</v>
-      </c>
-      <c r="C83" s="10" t="s">
-        <v>323</v>
       </c>
       <c r="D83" s="10">
         <v>1.318074</v>
@@ -4492,18 +4577,18 @@
         <v>103.89245200000001</v>
       </c>
       <c r="G83" s="7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84" t="s">
+      <c r="B84" t="s">
         <v>325</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" s="10" t="s">
         <v>326</v>
-      </c>
-      <c r="C84" s="10" t="s">
-        <v>327</v>
       </c>
       <c r="D84" s="10">
         <v>1.3265690000000001</v>
@@ -4515,18 +4600,18 @@
         <v>378961</v>
       </c>
       <c r="G84" s="7" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="85" spans="1:7">
-      <c r="A85" t="s">
+      <c r="B85" t="s">
         <v>329</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" s="10" t="s">
         <v>330</v>
-      </c>
-      <c r="C85" s="10" t="s">
-        <v>331</v>
       </c>
       <c r="D85" s="10">
         <v>1.335836</v>
@@ -4538,18 +4623,18 @@
         <v>369522</v>
       </c>
       <c r="G85" s="7" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="86" spans="1:7">
-      <c r="A86" t="s">
+      <c r="B86" t="s">
         <v>333</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" s="10" t="s">
         <v>334</v>
-      </c>
-      <c r="C86" s="10" t="s">
-        <v>335</v>
       </c>
       <c r="D86" s="10">
         <v>1.3427009999999999</v>
@@ -4561,18 +4646,18 @@
         <v>539788</v>
       </c>
       <c r="G86" s="7" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87" t="s">
-        <v>337</v>
-      </c>
       <c r="B87" t="s">
+        <v>258</v>
+      </c>
+      <c r="C87" s="10" t="s">
         <v>259</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>260</v>
       </c>
       <c r="D87" s="10">
         <v>1.3491789999999999</v>
@@ -4584,18 +4669,18 @@
         <v>534801</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>337</v>
+      </c>
+      <c r="B88" t="s">
         <v>338</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" s="10" t="s">
         <v>339</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>340</v>
       </c>
       <c r="D88" s="10">
         <v>1.352182</v>
@@ -4607,18 +4692,18 @@
         <v>556743</v>
       </c>
       <c r="G88" s="7" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89" t="s">
-        <v>342</v>
-      </c>
       <c r="B89" t="s">
+        <v>179</v>
+      </c>
+      <c r="C89" s="10" t="s">
         <v>180</v>
-      </c>
-      <c r="C89" s="10" t="s">
-        <v>181</v>
       </c>
       <c r="D89" s="10">
         <v>1.3507670000000001</v>
@@ -4630,18 +4715,18 @@
         <v>579827</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>342</v>
+      </c>
+      <c r="B90" t="s">
         <v>343</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" s="10" t="s">
         <v>344</v>
-      </c>
-      <c r="C90" s="10" t="s">
-        <v>345</v>
       </c>
       <c r="D90" s="10">
         <v>1.3490869999999999</v>
@@ -4653,18 +4738,18 @@
         <v>573993</v>
       </c>
       <c r="G90" s="7" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="91" spans="1:7">
-      <c r="A91" t="s">
+      <c r="B91" t="s">
         <v>347</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" s="10" t="s">
         <v>348</v>
-      </c>
-      <c r="C91" s="10" t="s">
-        <v>349</v>
       </c>
       <c r="D91" s="10">
         <v>1.337804</v>
@@ -4676,18 +4761,18 @@
         <v>298113</v>
       </c>
       <c r="G91" s="7" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="92" spans="1:7">
-      <c r="A92" t="s">
+      <c r="B92" t="s">
         <v>351</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" s="10" t="s">
         <v>352</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>353</v>
       </c>
       <c r="D92" s="10">
         <v>1.3225089999999999</v>
@@ -4696,15 +4781,15 @@
         <v>103.815376</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>353</v>
+      </c>
+      <c r="B93" t="s">
         <v>354</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" s="10" t="s">
         <v>355</v>
-      </c>
-      <c r="C93" s="10" t="s">
-        <v>356</v>
       </c>
       <c r="D93" s="10">
         <v>1.3173170000000001</v>
@@ -4716,18 +4801,18 @@
         <v>268857</v>
       </c>
       <c r="G93" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="A94" t="s">
+      <c r="B94" t="s">
         <v>358</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" s="10" t="s">
         <v>359</v>
-      </c>
-      <c r="C94" s="10" t="s">
-        <v>360</v>
       </c>
       <c r="D94" s="10">
         <v>1.3121259999999999</v>
@@ -4739,15 +4824,15 @@
         <v>268585</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>360</v>
+      </c>
+      <c r="B95" t="s">
         <v>361</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" s="10" t="s">
         <v>362</v>
-      </c>
-      <c r="C95" s="10" t="s">
-        <v>363</v>
       </c>
       <c r="D95" s="10">
         <v>1.3074490000000001</v>
@@ -4759,18 +4844,18 @@
         <v>139237</v>
       </c>
       <c r="G95" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="96" spans="1:7">
-      <c r="A96" t="s">
+      <c r="B96" t="s">
         <v>365</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" s="10" t="s">
         <v>366</v>
-      </c>
-      <c r="C96" s="10" t="s">
-        <v>367</v>
       </c>
       <c r="D96" s="10">
         <v>1.2992969999999999</v>
@@ -4779,18 +4864,18 @@
         <v>103.78709499999999</v>
       </c>
       <c r="G96" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97" t="s">
+      <c r="B97" t="s">
         <v>369</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" s="10" t="s">
         <v>370</v>
-      </c>
-      <c r="C97" s="10" t="s">
-        <v>371</v>
       </c>
       <c r="D97" s="10">
         <v>1.293377</v>
@@ -4799,18 +4884,18 @@
         <v>103.78434799999999</v>
       </c>
       <c r="G97" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="98" spans="1:7">
-      <c r="A98" t="s">
+      <c r="B98" t="s">
         <v>373</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" s="10" t="s">
         <v>374</v>
-      </c>
-      <c r="C98" s="10" t="s">
-        <v>375</v>
       </c>
       <c r="D98" s="10">
         <v>1.2823770000000001</v>
@@ -4819,18 +4904,18 @@
         <v>103.78187699999999</v>
       </c>
       <c r="G98" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="99" spans="1:7">
-      <c r="A99" t="s">
+      <c r="B99" t="s">
         <v>377</v>
       </c>
-      <c r="B99" t="s">
-        <v>378</v>
-      </c>
       <c r="C99" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D99" s="10">
         <v>1.2760640000000001</v>
@@ -4842,18 +4927,18 @@
         <v>118543</v>
       </c>
       <c r="G99" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="100" spans="1:7">
-      <c r="A100" t="s">
+      <c r="B100" t="s">
         <v>380</v>
       </c>
-      <c r="B100" t="s">
-        <v>381</v>
-      </c>
       <c r="C100" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D100" s="10">
         <v>1.272289</v>
@@ -4865,18 +4950,18 @@
         <v>109029</v>
       </c>
       <c r="G100" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="101" spans="1:7">
-      <c r="A101" t="s">
+      <c r="B101" t="s">
         <v>385</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" s="10" t="s">
         <v>386</v>
-      </c>
-      <c r="C101" s="10" t="s">
-        <v>387</v>
       </c>
       <c r="D101" s="10">
         <v>1.2705630000000001</v>
@@ -4885,18 +4970,18 @@
         <v>103.809577</v>
       </c>
       <c r="F101" s="13" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="102" spans="1:7">
-      <c r="A102" t="s">
+      <c r="B102" t="s">
         <v>389</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" s="10" t="s">
         <v>390</v>
-      </c>
-      <c r="C102" s="10" t="s">
-        <v>391</v>
       </c>
       <c r="D102" s="10">
         <v>1.2653719999999999</v>
@@ -4905,21 +4990,21 @@
         <v>103.82032700000001</v>
       </c>
       <c r="F102" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="G102" s="7" t="s">
         <v>392</v>
       </c>
-      <c r="G102" s="7" t="s">
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="103" spans="1:7">
-      <c r="A103" t="s">
+      <c r="B103" t="s">
         <v>394</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" s="10" t="s">
         <v>395</v>
-      </c>
-      <c r="C103" s="10" t="s">
-        <v>396</v>
       </c>
       <c r="D103" s="10">
         <v>1.282362</v>
@@ -4928,21 +5013,21 @@
         <v>103.858994</v>
       </c>
       <c r="F103" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="G103" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="G103" s="7" t="s">
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="104" spans="1:7">
-      <c r="A104" t="s">
+      <c r="B104" t="s">
         <v>399</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" s="10" t="s">
         <v>400</v>
-      </c>
-      <c r="C104" s="10" t="s">
-        <v>401</v>
       </c>
       <c r="D104" s="10">
         <v>1.276162</v>
@@ -4951,21 +5036,21 @@
         <v>103.854316</v>
       </c>
       <c r="F104" s="13" t="s">
+        <v>401</v>
+      </c>
+      <c r="G104" s="7" t="s">
         <v>402</v>
       </c>
-      <c r="G104" s="7" t="s">
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="105" spans="1:7">
-      <c r="A105" t="s">
+      <c r="B105" t="s">
         <v>404</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" s="10" t="s">
         <v>405</v>
-      </c>
-      <c r="C105" s="10" t="s">
-        <v>406</v>
       </c>
       <c r="D105" s="10">
         <v>1.300799</v>
@@ -4974,18 +5059,18 @@
         <v>103.85553400000001</v>
       </c>
       <c r="G105" s="7" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="106" spans="1:7">
-      <c r="A106" t="s">
+      <c r="B106" t="s">
         <v>408</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" s="10" t="s">
         <v>409</v>
-      </c>
-      <c r="C106" s="10" t="s">
-        <v>410</v>
       </c>
       <c r="D106" s="10">
         <v>1.2932049999999999</v>
@@ -4994,21 +5079,21 @@
         <v>103.861628</v>
       </c>
       <c r="F106" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="G106" s="7" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>412</v>
       </c>
-      <c r="G106" s="7" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7">
-      <c r="A107" t="s">
+      <c r="B107" t="s">
         <v>413</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" s="10" t="s">
         <v>414</v>
-      </c>
-      <c r="C107" s="10" t="s">
-        <v>415</v>
       </c>
       <c r="D107" s="10">
         <v>1.2824340000000001</v>
@@ -5017,21 +5102,21 @@
         <v>103.859549</v>
       </c>
       <c r="F107" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="G107" t="s">
         <v>416</v>
       </c>
-      <c r="G107" t="s">
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>420</v>
+      </c>
+      <c r="B108" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="108" spans="1:7">
-      <c r="A108" t="s">
-        <v>421</v>
-      </c>
-      <c r="B108" t="s">
+      <c r="C108" s="10" t="s">
         <v>418</v>
-      </c>
-      <c r="C108" s="10" t="s">
-        <v>419</v>
       </c>
       <c r="D108" s="10">
         <v>1.279401</v>
@@ -5040,18 +5125,18 @@
         <v>103.852964</v>
       </c>
       <c r="G108" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
+        <v>421</v>
+      </c>
+      <c r="B109" t="s">
         <v>422</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" s="10" t="s">
         <v>423</v>
-      </c>
-      <c r="C109" s="10" t="s">
-        <v>424</v>
       </c>
       <c r="D109" s="10">
         <v>1.2820450000000001</v>
@@ -5060,21 +5145,21 @@
         <v>103.848457</v>
       </c>
       <c r="F109" s="13" t="s">
+        <v>424</v>
+      </c>
+      <c r="G109" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="G109" s="7" t="s">
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="110" spans="1:7">
-      <c r="A110" t="s">
+      <c r="B110" t="s">
         <v>427</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" s="10" t="s">
         <v>428</v>
-      </c>
-      <c r="C110" s="10" t="s">
-        <v>429</v>
       </c>
       <c r="D110" s="10">
         <v>1.2844370000000001</v>
@@ -5083,21 +5168,21 @@
         <v>103.843264</v>
       </c>
       <c r="F110" s="13" t="s">
+        <v>429</v>
+      </c>
+      <c r="G110" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="G110" s="7" t="s">
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="A111" t="s">
+      <c r="B111" t="s">
         <v>432</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" s="10" t="s">
         <v>433</v>
-      </c>
-      <c r="C111" s="10" t="s">
-        <v>434</v>
       </c>
       <c r="D111" s="10">
         <v>1.385521</v>
@@ -5109,18 +5194,18 @@
         <v>689811</v>
       </c>
       <c r="G111" s="7" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="112" spans="1:7">
-      <c r="A112" t="s">
+      <c r="B112" t="s">
         <v>436</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" s="10" t="s">
         <v>437</v>
-      </c>
-      <c r="C112" s="10" t="s">
-        <v>438</v>
       </c>
       <c r="D112" s="10">
         <v>1.3803289999999999</v>
@@ -5132,18 +5217,18 @@
         <v>688265</v>
       </c>
       <c r="G112" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="113" spans="1:7">
-      <c r="A113" t="s">
+      <c r="B113" t="s">
         <v>440</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" s="10" t="s">
         <v>441</v>
-      </c>
-      <c r="C113" s="10" t="s">
-        <v>442</v>
       </c>
       <c r="D113" s="10">
         <v>1.3786560000000001</v>
@@ -5155,18 +5240,18 @@
         <v>688266</v>
       </c>
       <c r="G113" s="7" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="114" spans="1:7">
-      <c r="A114" t="s">
+      <c r="B114" t="s">
         <v>444</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" s="10" t="s">
         <v>445</v>
-      </c>
-      <c r="C114" s="10" t="s">
-        <v>446</v>
       </c>
       <c r="D114" s="10">
         <v>1.376811</v>
@@ -5178,18 +5263,18 @@
         <v>688267</v>
       </c>
       <c r="G114" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="115" spans="1:7">
-      <c r="A115" t="s">
+      <c r="B115" t="s">
         <v>448</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" s="10" t="s">
         <v>449</v>
-      </c>
-      <c r="C115" s="10" t="s">
-        <v>450</v>
       </c>
       <c r="D115" s="10">
         <v>1.3784419999999999</v>
@@ -5201,18 +5286,18 @@
         <v>689483</v>
       </c>
       <c r="G115" s="7" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="116" spans="1:7">
-      <c r="A116" t="s">
+      <c r="B116" t="s">
         <v>452</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" s="10" t="s">
         <v>453</v>
-      </c>
-      <c r="C116" s="10" t="s">
-        <v>454</v>
       </c>
       <c r="D116" s="10">
         <v>1.3781969999999999</v>
@@ -5224,18 +5309,18 @@
         <v>678270</v>
       </c>
       <c r="G116" s="7" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="117" spans="1:7">
-      <c r="A117" t="s">
+      <c r="B117" t="s">
         <v>456</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" s="10" t="s">
         <v>457</v>
-      </c>
-      <c r="C117" s="10" t="s">
-        <v>458</v>
       </c>
       <c r="D117" s="10">
         <v>1.377291</v>
@@ -5244,18 +5329,18 @@
         <v>103.767376</v>
       </c>
       <c r="G117" s="7" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="118" spans="1:7">
-      <c r="A118" t="s">
+      <c r="B118" t="s">
         <v>460</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" s="10" t="s">
         <v>461</v>
-      </c>
-      <c r="C118" s="10" t="s">
-        <v>462</v>
       </c>
       <c r="D118" s="10">
         <v>1.376261</v>
@@ -5264,18 +5349,18 @@
         <v>103.77131300000001</v>
       </c>
       <c r="G118" s="7" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="119" spans="1:7">
-      <c r="A119" t="s">
+      <c r="B119" t="s">
         <v>464</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" s="10" t="s">
         <v>465</v>
-      </c>
-      <c r="C119" s="10" t="s">
-        <v>466</v>
       </c>
       <c r="D119" s="10">
         <v>1.3803909999999999</v>
@@ -5287,18 +5372,18 @@
         <v>679939</v>
       </c>
       <c r="G119" s="7" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="120" spans="1:7">
-      <c r="A120" t="s">
+      <c r="B120" t="s">
         <v>468</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" s="10" t="s">
         <v>469</v>
-      </c>
-      <c r="C120" s="10" t="s">
-        <v>470</v>
       </c>
       <c r="D120" s="10">
         <v>1.3847449999999999</v>
@@ -5310,18 +5395,18 @@
         <v>679004</v>
       </c>
       <c r="G120" s="7" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="121" spans="1:7">
-      <c r="A121" t="s">
+      <c r="B121" t="s">
         <v>472</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" s="10" t="s">
         <v>473</v>
-      </c>
-      <c r="C121" s="10" t="s">
-        <v>474</v>
       </c>
       <c r="D121" s="10">
         <v>1.387491</v>
@@ -5333,18 +5418,18 @@
         <v>679940</v>
       </c>
       <c r="G121" s="7" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="122" spans="1:7">
-      <c r="A122" t="s">
+      <c r="B122" t="s">
         <v>476</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" s="10" t="s">
         <v>477</v>
-      </c>
-      <c r="C122" s="10" t="s">
-        <v>478</v>
       </c>
       <c r="D122" s="10">
         <v>1.3868050000000001</v>
@@ -5356,18 +5441,18 @@
         <v>679941</v>
       </c>
       <c r="G122" s="7" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="123" spans="1:7">
-      <c r="A123" t="s">
+      <c r="B123" t="s">
         <v>480</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" s="10" t="s">
         <v>481</v>
-      </c>
-      <c r="C123" s="10" t="s">
-        <v>482</v>
       </c>
       <c r="D123" s="10">
         <v>1.383211</v>
@@ -5376,18 +5461,18 @@
         <v>103.76216100000001</v>
       </c>
       <c r="G123" s="7" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="124" spans="1:7">
-      <c r="A124" t="s">
+      <c r="B124" t="s">
         <v>484</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>485</v>
-      </c>
-      <c r="C124" t="s">
-        <v>486</v>
       </c>
       <c r="D124">
         <v>1.4047289999999999</v>
@@ -5399,18 +5484,18 @@
         <v>828868</v>
       </c>
       <c r="G124" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="125" spans="1:7">
-      <c r="A125" t="s">
+      <c r="B125" t="s">
         <v>488</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>489</v>
-      </c>
-      <c r="C125" t="s">
-        <v>490</v>
       </c>
       <c r="D125">
         <v>1.3993370000000001</v>
@@ -5422,18 +5507,18 @@
         <v>820198</v>
       </c>
       <c r="G125" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="126" spans="1:7">
-      <c r="A126" t="s">
+      <c r="B126" t="s">
         <v>492</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>493</v>
-      </c>
-      <c r="C126" t="s">
-        <v>494</v>
       </c>
       <c r="D126">
         <v>1.3969780000000001</v>
@@ -5442,18 +5527,18 @@
         <v>103.909177</v>
       </c>
       <c r="G126" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="127" spans="1:7">
-      <c r="A127" t="s">
+      <c r="B127" t="s">
         <v>496</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" t="s">
         <v>497</v>
-      </c>
-      <c r="C127" t="s">
-        <v>498</v>
       </c>
       <c r="D127">
         <v>1.393448</v>
@@ -5462,18 +5547,18 @@
         <v>103.91209600000001</v>
       </c>
       <c r="G127" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="128" spans="1:7">
-      <c r="A128" t="s">
+      <c r="B128" t="s">
         <v>500</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" t="s">
         <v>501</v>
-      </c>
-      <c r="C128" t="s">
-        <v>502</v>
       </c>
       <c r="D128">
         <v>1.3946190000000001</v>
@@ -5485,18 +5570,18 @@
         <v>828852</v>
       </c>
       <c r="G128" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="129" spans="1:7">
-      <c r="A129" t="s">
+      <c r="B129" t="s">
         <v>504</v>
       </c>
-      <c r="B129" t="s">
+      <c r="C129" t="s">
         <v>505</v>
-      </c>
-      <c r="C129" t="s">
-        <v>506</v>
       </c>
       <c r="D129">
         <v>1.399338</v>
@@ -5508,18 +5593,18 @@
         <v>828853</v>
       </c>
       <c r="G129" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="130" spans="1:7">
-      <c r="A130" t="s">
+      <c r="B130" t="s">
         <v>508</v>
       </c>
-      <c r="B130" t="s">
+      <c r="C130" t="s">
         <v>509</v>
-      </c>
-      <c r="C130" t="s">
-        <v>510</v>
       </c>
       <c r="D130">
         <v>1.4016120000000001</v>
@@ -5528,18 +5613,18 @@
         <v>103.913605</v>
       </c>
       <c r="G130" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="131" spans="1:7">
-      <c r="A131" t="s">
+      <c r="B131" t="s">
         <v>512</v>
       </c>
-      <c r="B131" t="s">
+      <c r="C131" t="s">
         <v>513</v>
-      </c>
-      <c r="C131" t="s">
-        <v>514</v>
       </c>
       <c r="D131">
         <v>1.4053450000000001</v>
@@ -5551,18 +5636,18 @@
         <v>822612</v>
       </c>
       <c r="G131" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="132" spans="1:7">
-      <c r="A132" t="s">
+      <c r="B132" t="s">
         <v>516</v>
       </c>
-      <c r="B132" t="s">
+      <c r="C132" t="s">
         <v>517</v>
-      </c>
-      <c r="C132" t="s">
-        <v>518</v>
       </c>
       <c r="D132">
         <v>1.391745</v>
@@ -5574,18 +5659,18 @@
         <v>545062</v>
       </c>
       <c r="G132" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="133" spans="1:7">
-      <c r="A133" t="s">
+      <c r="B133" t="s">
         <v>520</v>
       </c>
-      <c r="B133" t="s">
+      <c r="C133" t="s">
         <v>521</v>
-      </c>
-      <c r="C133" t="s">
-        <v>522</v>
       </c>
       <c r="D133">
         <v>1.3946190000000001</v>
@@ -5597,18 +5682,18 @@
         <v>540250</v>
       </c>
       <c r="G133" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="134" spans="1:7">
-      <c r="A134" t="s">
+      <c r="B134" t="s">
         <v>524</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>525</v>
-      </c>
-      <c r="C134" t="s">
-        <v>526</v>
       </c>
       <c r="D134">
         <v>1.3911009999999999</v>
@@ -5617,18 +5702,18 @@
         <v>103.90622399999999</v>
       </c>
       <c r="G134" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="135" spans="1:7">
-      <c r="A135" t="s">
+      <c r="B135" t="s">
         <v>528</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C135" t="s">
         <v>529</v>
-      </c>
-      <c r="C135" t="s">
-        <v>530</v>
       </c>
       <c r="D135">
         <v>1.387883</v>
@@ -5640,18 +5725,18 @@
         <v>545053</v>
       </c>
       <c r="G135" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="136" spans="1:7">
-      <c r="A136" t="s">
+      <c r="B136" t="s">
         <v>532</v>
       </c>
-      <c r="B136" t="s">
+      <c r="C136" t="s">
         <v>533</v>
-      </c>
-      <c r="C136" t="s">
-        <v>534</v>
       </c>
       <c r="D136">
         <v>1.3837219999999999</v>
@@ -5663,18 +5748,18 @@
         <v>545052</v>
       </c>
       <c r="G136" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="137" spans="1:7">
-      <c r="A137" t="s">
+      <c r="B137" t="s">
         <v>536</v>
       </c>
-      <c r="B137" t="s">
+      <c r="C137" t="s">
         <v>537</v>
-      </c>
-      <c r="C137" t="s">
-        <v>538</v>
       </c>
       <c r="D137">
         <v>1.3836360000000001</v>
@@ -5683,18 +5768,18 @@
         <v>103.89764099999999</v>
       </c>
       <c r="G137" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="138" spans="1:7">
-      <c r="A138" t="s">
+      <c r="B138" t="s">
         <v>540</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" t="s">
         <v>541</v>
-      </c>
-      <c r="C138" t="s">
-        <v>542</v>
       </c>
       <c r="D138">
         <v>1.397295</v>
@@ -5706,18 +5791,18 @@
         <v>545048</v>
       </c>
       <c r="G138" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="139" spans="1:7">
-      <c r="A139" t="s">
+      <c r="B139" t="s">
         <v>544</v>
       </c>
-      <c r="B139" t="s">
+      <c r="C139" t="s">
         <v>545</v>
-      </c>
-      <c r="C139" t="s">
-        <v>546</v>
       </c>
       <c r="D139">
         <v>1.397348</v>
@@ -5729,18 +5814,18 @@
         <v>797699</v>
       </c>
       <c r="G139" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="140" spans="1:7">
-      <c r="A140" t="s">
+      <c r="B140" t="s">
         <v>548</v>
       </c>
-      <c r="B140" t="s">
+      <c r="C140" t="s">
         <v>549</v>
-      </c>
-      <c r="C140" t="s">
-        <v>550</v>
       </c>
       <c r="D140">
         <v>1.391921</v>
@@ -5752,18 +5837,18 @@
         <v>797698</v>
       </c>
       <c r="G140" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="141" spans="1:7">
-      <c r="A141" t="s">
+      <c r="B141" t="s">
         <v>552</v>
       </c>
-      <c r="B141" t="s">
+      <c r="C141" t="s">
         <v>553</v>
-      </c>
-      <c r="C141" t="s">
-        <v>554</v>
       </c>
       <c r="D141">
         <v>1.3921570000000001</v>
@@ -5775,18 +5860,18 @@
         <v>797700</v>
       </c>
       <c r="G141" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="142" spans="1:7">
-      <c r="A142" t="s">
+      <c r="B142" t="s">
         <v>556</v>
       </c>
-      <c r="B142" t="s">
+      <c r="C142" t="s">
         <v>557</v>
-      </c>
-      <c r="C142" t="s">
-        <v>558</v>
       </c>
       <c r="D142">
         <v>1.3892610000000001</v>
@@ -5798,18 +5883,18 @@
         <v>545050</v>
       </c>
       <c r="G142" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="143" spans="1:7">
-      <c r="A143" t="s">
+      <c r="B143" t="s">
         <v>560</v>
       </c>
-      <c r="B143" t="s">
+      <c r="C143" t="s">
         <v>561</v>
-      </c>
-      <c r="C143" t="s">
-        <v>562</v>
       </c>
       <c r="D143">
         <v>1.386644</v>
@@ -5821,7 +5906,199 @@
         <v>545049</v>
       </c>
       <c r="G143" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>565</v>
+      </c>
+      <c r="B144" t="s">
+        <v>575</v>
+      </c>
+      <c r="C144" s="10" t="s">
+        <v>453</v>
+      </c>
+      <c r="D144" s="10">
+        <v>1.3781969999999999</v>
+      </c>
+      <c r="E144" s="7">
+        <v>103.76354499999999</v>
+      </c>
+      <c r="F144">
+        <v>678270</v>
+      </c>
+      <c r="G144" s="7" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>566</v>
+      </c>
+      <c r="B145" t="s">
+        <v>576</v>
+      </c>
+      <c r="D145" s="16">
+        <v>1.3689750000000001</v>
+      </c>
+      <c r="E145" s="7">
+        <v>103.764803</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>567</v>
+      </c>
+      <c r="B146" t="s">
+        <v>577</v>
+      </c>
+      <c r="D146" s="16">
+        <v>1.3624719999999999</v>
+      </c>
+      <c r="E146" s="7">
+        <v>103.76738899999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>568</v>
+      </c>
+      <c r="B147" t="s">
+        <v>578</v>
+      </c>
+      <c r="D147" s="16">
+        <v>1.3411329999999999</v>
+      </c>
+      <c r="E147" s="7">
+        <v>103.775797</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>569</v>
+      </c>
+      <c r="B148" t="s">
+        <v>579</v>
+      </c>
+      <c r="D148" s="16">
+        <v>1.335628</v>
+      </c>
+      <c r="E148" s="7">
+        <v>103.78398300000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>570</v>
+      </c>
+      <c r="B149" t="s">
+        <v>580</v>
+      </c>
+      <c r="D149" s="16">
+        <v>1.330714</v>
+      </c>
+      <c r="E149" s="7">
+        <v>103.797633</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>571</v>
+      </c>
+      <c r="B150" t="s">
+        <v>581</v>
+      </c>
+      <c r="D150" s="16">
+        <v>1.326039</v>
+      </c>
+      <c r="E150" s="7">
+        <v>103.807169</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>572</v>
+      </c>
+      <c r="B151" t="s">
+        <v>582</v>
+      </c>
+      <c r="C151" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="D151" s="10">
+        <v>1.3225089999999999</v>
+      </c>
+      <c r="E151" s="7">
+        <v>103.815376</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>573</v>
+      </c>
+      <c r="B152" t="s">
+        <v>583</v>
+      </c>
+      <c r="D152" s="16">
+        <v>1.3200689999999999</v>
+      </c>
+      <c r="E152" s="7">
+        <v>103.825997</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>574</v>
+      </c>
+      <c r="B153" t="s">
+        <v>584</v>
+      </c>
+      <c r="C153" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D153">
+        <v>1.312487</v>
+      </c>
+      <c r="E153" s="7">
+        <v>103.837924</v>
+      </c>
+      <c r="F153">
+        <v>228234</v>
+      </c>
+      <c r="G153" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>564</v>
+      </c>
+      <c r="B154" t="s">
+        <v>585</v>
+      </c>
+      <c r="C154" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D154" s="10">
+        <v>1.3072280000000001</v>
+      </c>
+      <c r="E154" s="7">
+        <v>103.849847</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
         <v>563</v>
+      </c>
+      <c r="B155" t="s">
+        <v>586</v>
+      </c>
+      <c r="D155" s="16">
+        <v>1.3037639999999999</v>
+      </c>
+      <c r="E155" s="7">
+        <v>103.852581</v>
       </c>
     </row>
   </sheetData>
@@ -5837,7 +6114,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5850,7 +6127,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rewrite busstop process module
</commit_message>
<xml_diff>
--- a/inputdata/MRT.xlsx
+++ b/inputdata/MRT.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiangnanqing/Dropbox/project/busstoppy/inputdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiang\Dropbox\project\busstoppy\inputdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="19545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -260,10 +260,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>中 ？鲁站</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>EW16</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2353,16 +2349,19 @@
   </si>
   <si>
     <t>兀兰站</t>
+  </si>
+  <si>
+    <t>中巴鲁站</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2381,14 +2380,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
@@ -2465,14 +2456,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -2496,7 +2484,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -2544,6 +2532,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2839,22 +2830,22 @@
   <dimension ref="A1:H155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" customWidth="1"/>
-    <col min="8" max="8" width="25.83203125" customWidth="1"/>
+    <col min="2" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="12.125" customWidth="1"/>
+    <col min="5" max="5" width="17.625" customWidth="1"/>
+    <col min="6" max="6" width="16.875" customWidth="1"/>
+    <col min="7" max="7" width="30.625" customWidth="1"/>
+    <col min="8" max="8" width="25.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2880,8 +2871,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
@@ -2903,8 +2894,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
@@ -2926,8 +2917,8 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="17" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
@@ -2946,8 +2937,8 @@
         <v>649846</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:8">
+      <c r="A5" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
@@ -2969,8 +2960,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" s="17" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
@@ -2992,8 +2983,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7" s="17" t="s">
         <v>18</v>
       </c>
       <c r="B7" t="s">
@@ -3015,8 +3006,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B8" t="s">
@@ -3038,8 +3029,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:8">
+      <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B9" t="s">
@@ -3048,25 +3039,25 @@
       <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>1.31134</v>
       </c>
       <c r="E9">
         <v>103.77868100000001</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="3"/>
       <c r="G9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:8">
+      <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D10">
@@ -3075,21 +3066,21 @@
       <c r="E10">
         <v>103.789861</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>139345</v>
       </c>
       <c r="G10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:8">
+      <c r="A11" s="17" t="s">
         <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D11">
@@ -3098,21 +3089,21 @@
       <c r="E11">
         <v>103.79822900000001</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>149735</v>
       </c>
       <c r="G11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+    <row r="12" spans="1:8">
+      <c r="A12" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B12" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D12">
@@ -3121,19 +3112,19 @@
       <c r="E12">
         <v>103.80611500000001</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="4"/>
       <c r="G12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" s="17" t="s">
         <v>51</v>
       </c>
       <c r="B13" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D13">
@@ -3142,2391 +3133,2391 @@
       <c r="E13">
         <v>103.816715</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>158792</v>
       </c>
       <c r="G13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:8">
+      <c r="A14" s="17" t="s">
         <v>55</v>
       </c>
       <c r="B14" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>58</v>
+      <c r="C14" s="9" t="s">
+        <v>587</v>
       </c>
       <c r="D14">
         <v>1.286133</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>103.827079</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>168732</v>
       </c>
       <c r="G14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
+    <row r="15" spans="1:8">
+      <c r="A15" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
         <v>59</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>61</v>
       </c>
       <c r="D15" s="1">
         <v>1.28135</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>103.838838</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>169037</v>
       </c>
       <c r="G15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="17" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
+      <c r="B16" t="s">
         <v>63</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>65</v>
       </c>
       <c r="D16">
         <v>1.276491</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>103.845726</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="17" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
+      <c r="B17" t="s">
         <v>67</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>69</v>
       </c>
       <c r="D17">
         <v>1.283952</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>103.851281</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G17" s="7" t="s">
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="17" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+      <c r="B18" t="s">
         <v>72</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>74</v>
       </c>
       <c r="D18">
         <v>1.2932410000000001</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>103.852054</v>
       </c>
       <c r="F18">
         <v>179100</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="17" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+      <c r="B19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="B19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>77</v>
       </c>
       <c r="D19">
         <v>1.3007280000000001</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>103.856409</v>
       </c>
       <c r="F19">
         <v>188062</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="17" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
+      <c r="B20" t="s">
         <v>79</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>81</v>
       </c>
       <c r="D20">
         <v>1.307191</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>103.86299099999999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
+    <row r="21" spans="1:7">
+      <c r="A21" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" t="s">
         <v>82</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="9" t="s">
         <v>83</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>84</v>
       </c>
       <c r="D21">
         <v>1.311482</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>103.871392</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
+    <row r="22" spans="1:7">
+      <c r="A22" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" t="s">
         <v>85</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="9" t="s">
         <v>86</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>87</v>
       </c>
       <c r="D22">
         <v>1.3165119999999999</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>103.882893</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="18" t="s">
+    <row r="23" spans="1:7">
+      <c r="A23" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" t="s">
         <v>88</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" s="9" t="s">
         <v>89</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="D23">
         <v>1.3181210000000001</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="6">
         <v>103.89313900000001</v>
       </c>
       <c r="G23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="17" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
+      <c r="B24" t="s">
         <v>93</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" s="9" t="s">
         <v>94</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>95</v>
       </c>
       <c r="D24">
         <v>1.3197509999999999</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="6">
         <v>103.90310599999999</v>
       </c>
       <c r="F24">
         <v>409423</v>
       </c>
       <c r="G24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="17" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+      <c r="B25" t="s">
         <v>97</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>99</v>
       </c>
       <c r="D25">
         <v>1.3209630000000001</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="6">
         <v>103.912826</v>
       </c>
       <c r="F25">
         <v>416551</v>
       </c>
       <c r="G25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="17" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+      <c r="B26" t="s">
         <v>101</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" s="9" t="s">
         <v>102</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>103</v>
       </c>
       <c r="D26">
         <v>1.3240419999999999</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="6">
         <v>103.930025</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
+    <row r="27" spans="1:7">
+      <c r="A27" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" t="s">
         <v>104</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="9" t="s">
         <v>105</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>106</v>
       </c>
       <c r="D27">
         <v>1.3272569999999999</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="6">
         <v>103.946594</v>
       </c>
       <c r="F27">
         <v>467356</v>
       </c>
       <c r="G27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="17" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="18" t="s">
+      <c r="B28" t="s">
         <v>108</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>110</v>
       </c>
       <c r="D28">
         <v>1.343221</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="6">
         <v>103.953366</v>
       </c>
       <c r="F28">
         <v>489480</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="18" t="s">
+    <row r="29" spans="1:7">
+      <c r="A29" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" t="s">
         <v>111</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="D29" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D29" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" s="7">
+      <c r="E29" s="6">
         <v>103.945213</v>
       </c>
       <c r="F29">
         <v>529538</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="18" t="s">
+    <row r="30" spans="1:7">
+      <c r="A30" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" t="s">
         <v>115</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="9" t="s">
         <v>116</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>117</v>
       </c>
       <c r="D30">
         <v>1.3725449999999999</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="6">
         <v>103.949504</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" t="s">
         <v>118</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" s="9" t="s">
         <v>119</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>120</v>
       </c>
       <c r="D31">
         <v>1.3346929999999999</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="6">
         <v>103.96136199999999</v>
       </c>
       <c r="G31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
         <v>122</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>124</v>
       </c>
       <c r="D32">
         <v>1.357367</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="6">
         <v>103.988905</v>
       </c>
       <c r="G32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="18" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="19" t="s">
+      <c r="B33" t="s">
         <v>126</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" s="9" t="s">
         <v>127</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>128</v>
       </c>
       <c r="D33">
         <v>1.334362</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="6">
         <v>103.742569</v>
       </c>
       <c r="G33" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="18" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
+      <c r="B34" t="s">
         <v>130</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" s="9" t="s">
         <v>131</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>132</v>
       </c>
       <c r="D34">
         <v>1.3488629999999999</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="6">
         <v>103.749522</v>
       </c>
       <c r="G34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="18" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="19" t="s">
+      <c r="B35" t="s">
         <v>134</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" s="9" t="s">
         <v>135</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>136</v>
       </c>
       <c r="D35">
         <v>1.358903</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="6">
         <v>103.751839</v>
       </c>
       <c r="F35">
         <v>659083</v>
       </c>
       <c r="G35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="18" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="s">
+      <c r="B36" t="s">
         <v>138</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" s="9" t="s">
         <v>139</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>140</v>
       </c>
       <c r="D36">
         <v>1.3855630000000001</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="6">
         <v>103.74480699999999</v>
       </c>
       <c r="F36">
         <v>689810</v>
       </c>
       <c r="G36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="18" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
+      <c r="B37" t="s">
         <v>142</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>144</v>
       </c>
       <c r="D37">
         <v>1.3975759999999999</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="6">
         <v>103.747339</v>
       </c>
       <c r="F37">
         <v>689715</v>
       </c>
       <c r="G37" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="18" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="19" t="s">
+      <c r="B38" t="s">
         <v>146</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>148</v>
       </c>
       <c r="D38">
         <v>1.4250560000000001</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="6">
         <v>103.76190099999999</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="19" t="s">
+    <row r="39" spans="1:7">
+      <c r="A39" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" t="s">
         <v>149</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" s="9" t="s">
         <v>150</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>151</v>
       </c>
       <c r="D39">
         <v>1.432607</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="6">
         <v>103.774046</v>
       </c>
       <c r="F39">
         <v>739044</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="19" t="s">
+    <row r="40" spans="1:7">
+      <c r="A40" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B40" t="s">
         <v>152</v>
       </c>
-      <c r="B40" t="s">
-        <v>153</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>587</v>
+      <c r="C40" s="15" t="s">
+        <v>586</v>
       </c>
       <c r="D40">
         <v>1.4371970000000001</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="6">
         <v>103.786405</v>
       </c>
       <c r="F40">
         <v>738343</v>
       </c>
       <c r="G40" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="18" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="19" t="s">
+      <c r="B41" t="s">
         <v>155</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>157</v>
       </c>
       <c r="D41">
         <v>1.440715</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="6">
         <v>103.800997</v>
       </c>
       <c r="F41">
         <v>738344</v>
       </c>
       <c r="G41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="18" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="19" t="s">
+      <c r="B42" t="s">
         <v>159</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>161</v>
       </c>
       <c r="D42">
         <v>1.4490810000000001</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="6">
         <v>103.820223</v>
       </c>
       <c r="F42">
         <v>759775</v>
       </c>
       <c r="G42" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="18" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" s="19" t="s">
+      <c r="B43" t="s">
         <v>163</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>165</v>
       </c>
       <c r="D43">
         <v>1.4295610000000001</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="6">
         <v>103.83524300000001</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44" s="19" t="s">
+    <row r="44" spans="1:7">
+      <c r="A44" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B44" t="s">
         <v>166</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>168</v>
       </c>
       <c r="D44">
         <v>1.417548</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E44" s="13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="18" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" s="19" t="s">
+      <c r="B45" t="s">
         <v>170</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" s="9" t="s">
         <v>171</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>172</v>
       </c>
       <c r="D45">
         <v>1.3820790000000001</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="6">
         <v>103.844773</v>
       </c>
       <c r="F45">
         <v>569813</v>
       </c>
       <c r="G45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="18" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="19" t="s">
+      <c r="B46" t="s">
         <v>174</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>176</v>
       </c>
       <c r="D46">
         <v>1.3700349999999999</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46" s="6">
         <v>103.849475</v>
       </c>
       <c r="F46">
         <v>569811</v>
       </c>
       <c r="G46" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="18" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="19" t="s">
+      <c r="B47" t="s">
         <v>178</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" s="9" t="s">
         <v>179</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>180</v>
       </c>
       <c r="D47">
         <v>1.350803</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47" s="6">
         <v>103.848316</v>
       </c>
       <c r="F47">
         <v>579827</v>
       </c>
       <c r="G47" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="18" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="19" t="s">
+      <c r="B48" t="s">
         <v>182</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" s="9" t="s">
         <v>183</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>184</v>
       </c>
       <c r="D48">
         <v>1.340292</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48" s="6">
         <v>103.845215</v>
       </c>
       <c r="F48">
         <v>319758</v>
       </c>
       <c r="G48" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="18" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="19" t="s">
+      <c r="B49" t="s">
         <v>186</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" s="9" t="s">
         <v>187</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>188</v>
       </c>
       <c r="D49">
         <v>1.3327260000000001</v>
       </c>
-      <c r="E49" s="7">
+      <c r="E49" s="6">
         <v>103.84779399999999</v>
       </c>
       <c r="F49">
         <v>310190</v>
       </c>
       <c r="G49" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="18" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="19" t="s">
+      <c r="B50" t="s">
         <v>190</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" s="9" t="s">
         <v>191</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>192</v>
       </c>
       <c r="D50">
         <v>1.320038</v>
       </c>
-      <c r="E50" s="7">
+      <c r="E50" s="6">
         <v>103.843846</v>
       </c>
       <c r="F50">
         <v>307683</v>
       </c>
       <c r="G50" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="18" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" s="19" t="s">
+      <c r="B51" t="s">
         <v>194</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" s="9" t="s">
         <v>195</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>196</v>
       </c>
       <c r="D51">
         <v>1.312487</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51" s="6">
         <v>103.837924</v>
       </c>
       <c r="F51">
         <v>228234</v>
       </c>
       <c r="G51" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="18" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="19" t="s">
+      <c r="B52" t="s">
         <v>198</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" s="9" t="s">
         <v>199</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>200</v>
       </c>
       <c r="D52">
         <v>1.304324</v>
       </c>
-      <c r="E52" s="7">
+      <c r="E52" s="6">
         <v>103.83248399999999</v>
       </c>
       <c r="F52">
         <v>238801</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="19" t="s">
+    <row r="53" spans="1:7">
+      <c r="A53" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="B53" t="s">
         <v>201</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" s="9" t="s">
         <v>202</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>203</v>
       </c>
       <c r="D53">
         <v>1.300125</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E53" s="6">
         <v>103.838588</v>
       </c>
       <c r="F53">
         <v>238162</v>
       </c>
       <c r="G53" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="18" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="19" t="s">
+      <c r="B54" t="s">
         <v>205</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" s="9" t="s">
         <v>206</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>207</v>
       </c>
       <c r="D54">
         <v>1.2985910000000001</v>
       </c>
-      <c r="E54" s="7">
+      <c r="E54" s="6">
         <v>103.846191</v>
       </c>
       <c r="F54">
         <v>238826</v>
       </c>
       <c r="G54" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="18" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="19" t="s">
+      <c r="B55" t="s">
         <v>209</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" s="9" t="s">
         <v>210</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>211</v>
       </c>
       <c r="D55">
         <v>1.293239</v>
       </c>
-      <c r="E55" s="7">
+      <c r="E55" s="6">
         <v>103.85237100000001</v>
       </c>
       <c r="F55">
         <v>179100</v>
       </c>
       <c r="G55" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="18" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="19" t="s">
+      <c r="B56" t="s">
         <v>213</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" s="9" t="s">
         <v>214</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>215</v>
       </c>
       <c r="D56">
         <v>1.2839389999999999</v>
       </c>
-      <c r="E56" s="7">
+      <c r="E56" s="6">
         <v>103.851642</v>
       </c>
-      <c r="F56" s="13" t="s">
+      <c r="F56" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="18" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="19" t="s">
+      <c r="B57" t="s">
         <v>217</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="D57" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E57" s="6">
+        <v>103.85480699999999</v>
+      </c>
+      <c r="F57" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="G57" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="E57" s="7">
-        <v>103.85480699999999</v>
-      </c>
-      <c r="F57" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="19" t="s">
+      <c r="B58" t="s">
         <v>223</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" s="9" t="s">
         <v>224</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>225</v>
       </c>
       <c r="D58">
         <v>1.2709710000000001</v>
       </c>
-      <c r="E58" s="15" t="s">
+      <c r="E58" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="F58" s="13" t="s">
-        <v>227</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="20" t="s">
+      <c r="B59" t="s">
         <v>229</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>231</v>
       </c>
       <c r="D59">
         <v>1.2652969999999999</v>
       </c>
-      <c r="E59" s="7">
+      <c r="E59" s="6">
         <v>103.82118199999999</v>
       </c>
-      <c r="F59" s="13" t="s">
+      <c r="F59" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="G59" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="G59" s="7" t="s">
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="19" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="20" t="s">
+      <c r="B60" t="s">
         <v>234</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" s="9" t="s">
         <v>235</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>236</v>
       </c>
       <c r="D60">
         <v>1.281344</v>
       </c>
-      <c r="E60" s="7">
+      <c r="E60" s="6">
         <v>103.839765</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="20" t="s">
+    <row r="61" spans="1:7">
+      <c r="A61" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="B61" t="s">
         <v>237</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" s="9" t="s">
         <v>238</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>239</v>
       </c>
       <c r="D61">
         <v>1.284446</v>
       </c>
-      <c r="E61" s="7">
+      <c r="E61" s="6">
         <v>103.843559</v>
       </c>
-      <c r="F61" s="13"/>
+      <c r="F61" s="12"/>
       <c r="G61" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="B62" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="B62" t="s">
+      <c r="C62" s="9" t="s">
         <v>241</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>242</v>
       </c>
       <c r="D62">
         <v>1.2885009999999999</v>
       </c>
-      <c r="E62" s="7">
+      <c r="E62" s="6">
         <v>103.846778</v>
       </c>
       <c r="G62" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="20" t="s">
-        <v>262</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="19" t="s">
+        <v>261</v>
       </c>
       <c r="B63" t="s">
+        <v>205</v>
+      </c>
+      <c r="C63" s="9" t="s">
         <v>206</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>207</v>
       </c>
       <c r="D63">
         <v>1.298594</v>
       </c>
-      <c r="E63" s="7">
+      <c r="E63" s="6">
         <v>103.845888</v>
       </c>
       <c r="F63">
         <v>238826</v>
       </c>
       <c r="G63" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="20" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="B64" t="s">
+        <v>243</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D64" s="9">
+        <v>1.3072280000000001</v>
+      </c>
+      <c r="E64" s="6">
+        <v>103.849847</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="B64" t="s">
-        <v>244</v>
-      </c>
-      <c r="C64" s="10" t="s">
+      <c r="B65" t="s">
         <v>245</v>
       </c>
-      <c r="D64" s="10">
-        <v>1.3072280000000001</v>
-      </c>
-      <c r="E64" s="7">
-        <v>103.849847</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A65" s="20" t="s">
-        <v>264</v>
-      </c>
-      <c r="B65" t="s">
+      <c r="C65" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="C65" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="D65" s="10">
+      <c r="D65" s="9">
         <v>1.3124089999999999</v>
       </c>
-      <c r="E65" s="15" t="s">
-        <v>249</v>
+      <c r="E65" s="14" t="s">
+        <v>248</v>
       </c>
       <c r="F65">
         <v>217562</v>
       </c>
       <c r="G65" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66" s="20" t="s">
-        <v>265</v>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="19" t="s">
+        <v>264</v>
       </c>
       <c r="B66" t="s">
+        <v>249</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="C66" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="D66" s="10">
+      <c r="D66" s="9">
         <v>1.319596</v>
       </c>
-      <c r="E66" s="7">
+      <c r="E66" s="6">
         <v>103.861949</v>
       </c>
       <c r="F66">
         <v>328260</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A67" s="20" t="s">
-        <v>266</v>
+    <row r="67" spans="1:7">
+      <c r="A67" s="19" t="s">
+        <v>265</v>
       </c>
       <c r="B67" t="s">
-        <v>254</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="D67" s="10">
+        <v>253</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="D67" s="9">
         <v>1.3313619999999999</v>
       </c>
-      <c r="E67" s="7">
+      <c r="E67" s="6">
         <v>103.869276</v>
       </c>
       <c r="F67">
         <v>347663</v>
       </c>
       <c r="G67" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68" s="20" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="B68" t="s">
+        <v>254</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="D68" s="9">
+        <v>1.3393630000000001</v>
+      </c>
+      <c r="E68" s="6">
+        <v>103.870757</v>
+      </c>
+      <c r="G68" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="B68" t="s">
-        <v>255</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="D68" s="10">
-        <v>1.3393630000000001</v>
-      </c>
-      <c r="E68" s="7">
-        <v>103.870757</v>
-      </c>
-      <c r="G68" t="s">
+      <c r="B69" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A69" s="20" t="s">
-        <v>268</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="C69" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C69" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="D69" s="10">
+      <c r="D69" s="9">
         <v>1.3492420000000001</v>
       </c>
-      <c r="E69" s="7">
+      <c r="E69" s="6">
         <v>103.873632</v>
       </c>
       <c r="F69">
         <v>534801</v>
       </c>
       <c r="G69" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70" s="20" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="B70" t="s">
         <v>269</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="D70" s="9">
+        <v>1.3605149999999999</v>
+      </c>
+      <c r="E70" s="6">
+        <v>103.885209</v>
+      </c>
+      <c r="G70" t="s">
         <v>271</v>
       </c>
-      <c r="D70" s="10">
-        <v>1.3605149999999999</v>
-      </c>
-      <c r="E70" s="7">
-        <v>103.885209</v>
-      </c>
-      <c r="G70" t="s">
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="19" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A71" s="20" t="s">
+      <c r="B71" t="s">
         <v>273</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="C71" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="D71" s="10">
+      <c r="D71" s="9">
         <v>1.370919</v>
       </c>
-      <c r="E71" s="7">
+      <c r="E71" s="6">
         <v>103.892472</v>
       </c>
       <c r="F71">
         <v>538757</v>
       </c>
       <c r="G71" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="19" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72" s="20" t="s">
+      <c r="B72" t="s">
         <v>277</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="C72" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="D72" s="10">
+      <c r="D72" s="9">
         <v>1.382449</v>
       </c>
-      <c r="E72" s="7">
+      <c r="E72" s="6">
         <v>103.892719</v>
       </c>
       <c r="F72">
         <v>549927</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A73" s="20" t="s">
+    <row r="73" spans="1:7">
+      <c r="A73" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="B73" t="s">
+        <v>281</v>
+      </c>
+      <c r="C73" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="B73" t="s">
-        <v>282</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="D73" s="10">
+      <c r="D73" s="9">
         <v>1.3912659999999999</v>
       </c>
-      <c r="E73" s="7">
+      <c r="E73" s="6">
         <v>103.895369</v>
       </c>
       <c r="F73">
         <v>545062</v>
       </c>
       <c r="G73" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="19" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74" s="20" t="s">
+      <c r="B74" t="s">
         <v>284</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="C74" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="D74" s="10">
+      <c r="D74" s="9">
         <v>1.4045449999999999</v>
       </c>
-      <c r="E74" s="7">
+      <c r="E74" s="6">
         <v>103.902023</v>
       </c>
       <c r="F74">
         <v>828868</v>
       </c>
       <c r="G74" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" s="20" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="21" t="s">
+      <c r="B75" t="s">
+        <v>205</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="D75" s="9">
+        <v>1.298746</v>
+      </c>
+      <c r="E75" s="6">
+        <v>103.844688</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="B75" t="s">
-        <v>206</v>
-      </c>
-      <c r="C75" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="D75" s="10">
-        <v>1.298746</v>
-      </c>
-      <c r="E75" s="7">
-        <v>103.844688</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="21" t="s">
+      <c r="B76" t="s">
         <v>289</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="C76" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="D76" s="10">
+      <c r="D76" s="9">
         <v>1.2969440000000001</v>
       </c>
-      <c r="E76" s="7">
+      <c r="E76" s="6">
         <v>103.850739</v>
       </c>
       <c r="F76">
         <v>189561</v>
       </c>
       <c r="G76" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="20" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="21" t="s">
+      <c r="B77" t="s">
         <v>293</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="C77" s="10" t="s">
+      <c r="D77" s="9">
+        <v>1.2934680000000001</v>
+      </c>
+      <c r="E77" s="6">
+        <v>103.855352</v>
+      </c>
+      <c r="F77" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="D77" s="10">
-        <v>1.2934680000000001</v>
-      </c>
-      <c r="E77" s="7">
-        <v>103.855352</v>
-      </c>
-      <c r="F77" s="13" t="s">
+      <c r="G77" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="G77" s="7" t="s">
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="20" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="21" t="s">
+      <c r="B78" t="s">
         <v>298</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="C78" s="10" t="s">
+      <c r="D78" s="9">
+        <v>1.293147</v>
+      </c>
+      <c r="E78" s="6">
+        <v>103.86082399999999</v>
+      </c>
+      <c r="F78" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="G78" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="D78" s="10">
-        <v>1.293147</v>
-      </c>
-      <c r="E78" s="7">
-        <v>103.86082399999999</v>
-      </c>
-      <c r="F78" s="13" t="s">
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="20" t="s">
         <v>302</v>
       </c>
-      <c r="G78" s="7" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A79" s="21" t="s">
+      <c r="B79" t="s">
         <v>303</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="D79" s="9">
+        <v>1.2997540000000001</v>
+      </c>
+      <c r="E79" s="6">
+        <v>103.863699</v>
+      </c>
+      <c r="F79" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="D79" s="10">
-        <v>1.2997540000000001</v>
-      </c>
-      <c r="E79" s="7">
-        <v>103.863699</v>
-      </c>
-      <c r="F79" s="13" t="s">
+      <c r="G79" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="G79" s="7" t="s">
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="20" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A80" s="21" t="s">
+      <c r="B80" t="s">
         <v>308</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="C80" s="10" t="s">
-        <v>310</v>
-      </c>
-      <c r="D80" s="10">
+      <c r="D80" s="9">
         <v>1.302929</v>
       </c>
-      <c r="E80" s="7">
+      <c r="E80" s="6">
         <v>103.875286</v>
       </c>
       <c r="F80">
         <v>397692</v>
       </c>
-      <c r="G80" s="7" t="s">
+      <c r="G80" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="20" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A81" s="21" t="s">
+      <c r="B81" t="s">
         <v>312</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="C81" s="10" t="s">
+      <c r="D81" s="9">
+        <v>1.3064039999999999</v>
+      </c>
+      <c r="E81" s="6">
+        <v>103.882582</v>
+      </c>
+      <c r="G81" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="D81" s="10">
-        <v>1.3064039999999999</v>
-      </c>
-      <c r="E81" s="7">
-        <v>103.882582</v>
-      </c>
-      <c r="G81" s="7" t="s">
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="20" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A82" s="21" t="s">
+      <c r="B82" t="s">
         <v>316</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="C82" s="10" t="s">
+      <c r="D82" s="9">
+        <v>1.308292</v>
+      </c>
+      <c r="E82" s="6">
+        <v>103.88824700000001</v>
+      </c>
+      <c r="G82" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="D82" s="10">
-        <v>1.308292</v>
-      </c>
-      <c r="E82" s="7">
-        <v>103.88824700000001</v>
-      </c>
-      <c r="G82" s="7" t="s">
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="20" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83" s="21" t="s">
+      <c r="B83" t="s">
         <v>320</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="C83" s="10" t="s">
+      <c r="D83" s="9">
+        <v>1.318074</v>
+      </c>
+      <c r="E83" s="6">
+        <v>103.89245200000001</v>
+      </c>
+      <c r="G83" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="D83" s="10">
-        <v>1.318074</v>
-      </c>
-      <c r="E83" s="7">
-        <v>103.89245200000001</v>
-      </c>
-      <c r="G83" s="7" t="s">
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="20" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84" s="21" t="s">
+      <c r="B84" t="s">
         <v>324</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="C84" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="D84" s="10">
+      <c r="D84" s="9">
         <v>1.3265690000000001</v>
       </c>
-      <c r="E84" s="7">
+      <c r="E84" s="6">
         <v>103.890049</v>
       </c>
       <c r="F84">
         <v>378961</v>
       </c>
-      <c r="G84" s="7" t="s">
+      <c r="G84" s="6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="20" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85" s="21" t="s">
+      <c r="B85" t="s">
         <v>328</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="C85" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="D85" s="10">
+      <c r="D85" s="9">
         <v>1.335836</v>
       </c>
-      <c r="E85" s="7">
+      <c r="E85" s="6">
         <v>103.887861</v>
       </c>
       <c r="F85">
         <v>369522</v>
       </c>
-      <c r="G85" s="7" t="s">
+      <c r="G85" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="20" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86" s="21" t="s">
+      <c r="B86" t="s">
         <v>332</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="C86" s="10" t="s">
-        <v>334</v>
-      </c>
-      <c r="D86" s="10">
+      <c r="D86" s="9">
         <v>1.3427009999999999</v>
       </c>
-      <c r="E86" s="7">
+      <c r="E86" s="6">
         <v>103.879964</v>
       </c>
       <c r="F86">
         <v>539788</v>
       </c>
-      <c r="G86" s="7" t="s">
+      <c r="G86" s="6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="20" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87" s="21" t="s">
-        <v>336</v>
-      </c>
       <c r="B87" t="s">
+        <v>257</v>
+      </c>
+      <c r="C87" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="C87" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="D87" s="10">
+      <c r="D87" s="9">
         <v>1.3491789999999999</v>
       </c>
-      <c r="E87" s="7">
+      <c r="E87" s="6">
         <v>103.87279700000001</v>
       </c>
       <c r="F87">
         <v>534801</v>
       </c>
-      <c r="G87" s="7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88" s="21" t="s">
+      <c r="G87" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="B88" t="s">
         <v>337</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="C88" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="D88" s="10">
+      <c r="D88" s="9">
         <v>1.352182</v>
       </c>
-      <c r="E88" s="7">
+      <c r="E88" s="6">
         <v>103.863528</v>
       </c>
       <c r="F88">
         <v>556743</v>
       </c>
-      <c r="G88" s="7" t="s">
+      <c r="G88" s="6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="20" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89" s="21" t="s">
-        <v>341</v>
-      </c>
       <c r="B89" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C89" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="D89" s="10">
+      <c r="D89" s="9">
         <v>1.3507670000000001</v>
       </c>
-      <c r="E89" s="7">
+      <c r="E89" s="6">
         <v>103.847477</v>
       </c>
       <c r="F89">
         <v>579827</v>
       </c>
-      <c r="G89" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90" s="21" t="s">
+      <c r="G89" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="B90" t="s">
         <v>342</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="C90" s="10" t="s">
-        <v>344</v>
-      </c>
-      <c r="D90" s="10">
+      <c r="D90" s="9">
         <v>1.3490869999999999</v>
       </c>
-      <c r="E90" s="7">
+      <c r="E90" s="6">
         <v>103.839516</v>
       </c>
       <c r="F90">
         <v>573993</v>
       </c>
-      <c r="G90" s="7" t="s">
+      <c r="G90" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="20" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91" s="21" t="s">
+      <c r="B91" t="s">
         <v>346</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="C91" s="10" t="s">
-        <v>348</v>
-      </c>
-      <c r="D91" s="10">
+      <c r="D91" s="9">
         <v>1.337804</v>
       </c>
-      <c r="E91" s="7">
+      <c r="E91" s="6">
         <v>103.839473</v>
       </c>
       <c r="F91">
         <v>298113</v>
       </c>
-      <c r="G91" s="7" t="s">
+      <c r="G91" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="20" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92" s="21" t="s">
+      <c r="B92" t="s">
         <v>350</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="C92" s="10" t="s">
+      <c r="D92" s="9">
+        <v>1.3225089999999999</v>
+      </c>
+      <c r="E92" s="6">
+        <v>103.815376</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="20" t="s">
         <v>352</v>
       </c>
-      <c r="D92" s="10">
-        <v>1.3225089999999999</v>
-      </c>
-      <c r="E92" s="7">
-        <v>103.815376</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93" s="21" t="s">
+      <c r="B93" t="s">
         <v>353</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" s="9" t="s">
         <v>354</v>
       </c>
-      <c r="C93" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="D93" s="10">
+      <c r="D93" s="9">
         <v>1.3173170000000001</v>
       </c>
-      <c r="E93" s="7">
+      <c r="E93" s="6">
         <v>103.80743699999999</v>
       </c>
       <c r="F93">
         <v>268857</v>
       </c>
       <c r="G93" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" s="20" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94" s="21" t="s">
+      <c r="B94" t="s">
         <v>357</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="C94" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="D94" s="10">
+      <c r="D94" s="9">
         <v>1.3121259999999999</v>
       </c>
-      <c r="E94" s="7">
+      <c r="E94" s="6">
         <v>103.796193</v>
       </c>
       <c r="F94">
         <v>268585</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A95" s="21" t="s">
+    <row r="95" spans="1:7">
+      <c r="A95" s="20" t="s">
+        <v>359</v>
+      </c>
+      <c r="B95" t="s">
         <v>360</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="C95" s="10" t="s">
-        <v>362</v>
-      </c>
-      <c r="D95" s="10">
+      <c r="D95" s="9">
         <v>1.3074490000000001</v>
       </c>
-      <c r="E95" s="7">
+      <c r="E95" s="6">
         <v>103.788983</v>
       </c>
       <c r="F95">
         <v>139237</v>
       </c>
       <c r="G95" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" s="20" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96" s="21" t="s">
+      <c r="B96" t="s">
         <v>364</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="C96" s="10" t="s">
+      <c r="D96" s="9">
+        <v>1.2992969999999999</v>
+      </c>
+      <c r="E96" s="6">
+        <v>103.78709499999999</v>
+      </c>
+      <c r="G96" t="s">
         <v>366</v>
       </c>
-      <c r="D96" s="10">
-        <v>1.2992969999999999</v>
-      </c>
-      <c r="E96" s="7">
-        <v>103.78709499999999</v>
-      </c>
-      <c r="G96" t="s">
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" s="20" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97" s="21" t="s">
+      <c r="B97" t="s">
         <v>368</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="D97" s="9">
+        <v>1.293377</v>
+      </c>
+      <c r="E97" s="6">
+        <v>103.78434799999999</v>
+      </c>
+      <c r="G97" t="s">
         <v>370</v>
       </c>
-      <c r="D97" s="10">
-        <v>1.293377</v>
-      </c>
-      <c r="E97" s="7">
-        <v>103.78434799999999</v>
-      </c>
-      <c r="G97" t="s">
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" s="20" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98" s="21" t="s">
+      <c r="B98" t="s">
         <v>372</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="C98" s="10" t="s">
+      <c r="D98" s="9">
+        <v>1.2823770000000001</v>
+      </c>
+      <c r="E98" s="6">
+        <v>103.78187699999999</v>
+      </c>
+      <c r="G98" t="s">
         <v>374</v>
       </c>
-      <c r="D98" s="10">
-        <v>1.2823770000000001</v>
-      </c>
-      <c r="E98" s="7">
-        <v>103.78187699999999</v>
-      </c>
-      <c r="G98" t="s">
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" s="20" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A99" s="21" t="s">
+      <c r="B99" t="s">
         <v>376</v>
       </c>
-      <c r="B99" t="s">
-        <v>377</v>
-      </c>
-      <c r="C99" s="10" t="s">
-        <v>381</v>
-      </c>
-      <c r="D99" s="10">
+      <c r="C99" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="D99" s="9">
         <v>1.2760640000000001</v>
       </c>
-      <c r="E99" s="7">
+      <c r="E99" s="6">
         <v>103.791138</v>
       </c>
       <c r="F99">
         <v>118543</v>
       </c>
       <c r="G99" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" s="20" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A100" s="21" t="s">
+      <c r="B100" t="s">
         <v>379</v>
       </c>
-      <c r="B100" t="s">
-        <v>380</v>
-      </c>
-      <c r="C100" s="10" t="s">
-        <v>382</v>
-      </c>
-      <c r="D100" s="10">
+      <c r="C100" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="D100" s="9">
         <v>1.272289</v>
       </c>
-      <c r="E100" s="7">
+      <c r="E100" s="6">
         <v>103.80281100000001</v>
       </c>
       <c r="F100">
         <v>109029</v>
       </c>
       <c r="G100" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" s="20" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A101" s="21" t="s">
+      <c r="B101" t="s">
         <v>384</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="C101" s="10" t="s">
+      <c r="D101" s="9">
+        <v>1.2705630000000001</v>
+      </c>
+      <c r="E101" s="6">
+        <v>103.809577</v>
+      </c>
+      <c r="F101" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="D101" s="10">
-        <v>1.2705630000000001</v>
-      </c>
-      <c r="E101" s="7">
-        <v>103.809577</v>
-      </c>
-      <c r="F101" s="13" t="s">
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="20" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A102" s="21" t="s">
+      <c r="B102" t="s">
         <v>388</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="C102" s="10" t="s">
+      <c r="D102" s="9">
+        <v>1.2653719999999999</v>
+      </c>
+      <c r="E102" s="6">
+        <v>103.82032700000001</v>
+      </c>
+      <c r="F102" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="D102" s="10">
-        <v>1.2653719999999999</v>
-      </c>
-      <c r="E102" s="7">
-        <v>103.82032700000001</v>
-      </c>
-      <c r="F102" s="13" t="s">
+      <c r="G102" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="G102" s="7" t="s">
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="B103" t="s">
         <v>393</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="C103" s="10" t="s">
+      <c r="D103" s="9">
+        <v>1.282362</v>
+      </c>
+      <c r="E103" s="6">
+        <v>103.858994</v>
+      </c>
+      <c r="F103" s="12" t="s">
         <v>395</v>
       </c>
-      <c r="D103" s="10">
-        <v>1.282362</v>
-      </c>
-      <c r="E103" s="7">
-        <v>103.858994</v>
-      </c>
-      <c r="F103" s="13" t="s">
+      <c r="G103" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="G103" s="7" t="s">
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="B104" t="s">
         <v>398</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="C104" s="10" t="s">
+      <c r="D104" s="9">
+        <v>1.276162</v>
+      </c>
+      <c r="E104" s="6">
+        <v>103.854316</v>
+      </c>
+      <c r="F104" s="12" t="s">
         <v>400</v>
       </c>
-      <c r="D104" s="10">
-        <v>1.276162</v>
-      </c>
-      <c r="E104" s="7">
-        <v>103.854316</v>
-      </c>
-      <c r="F104" s="13" t="s">
+      <c r="G104" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="G104" s="7" t="s">
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" s="21" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A105" s="22" t="s">
+      <c r="B105" t="s">
         <v>403</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="C105" s="10" t="s">
+      <c r="D105" s="9">
+        <v>1.300799</v>
+      </c>
+      <c r="E105" s="6">
+        <v>103.85553400000001</v>
+      </c>
+      <c r="G105" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="D105" s="10">
-        <v>1.300799</v>
-      </c>
-      <c r="E105" s="7">
-        <v>103.85553400000001</v>
-      </c>
-      <c r="G105" s="7" t="s">
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" s="21" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A106" s="22" t="s">
+      <c r="B106" t="s">
         <v>407</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="C106" s="10" t="s">
+      <c r="D106" s="9">
+        <v>1.2932049999999999</v>
+      </c>
+      <c r="E106" s="6">
+        <v>103.861628</v>
+      </c>
+      <c r="F106" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="G106" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="D106" s="10">
-        <v>1.2932049999999999</v>
-      </c>
-      <c r="E106" s="7">
-        <v>103.861628</v>
-      </c>
-      <c r="F106" s="13" t="s">
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" s="21" t="s">
         <v>411</v>
       </c>
-      <c r="G106" s="7" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A107" s="22" t="s">
+      <c r="B107" t="s">
         <v>412</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="C107" s="10" t="s">
+      <c r="D107" s="9">
+        <v>1.2824340000000001</v>
+      </c>
+      <c r="E107" s="6">
+        <v>103.859549</v>
+      </c>
+      <c r="F107" s="12" t="s">
         <v>414</v>
       </c>
-      <c r="D107" s="10">
-        <v>1.2824340000000001</v>
-      </c>
-      <c r="E107" s="7">
-        <v>103.859549</v>
-      </c>
-      <c r="F107" s="13" t="s">
+      <c r="G107" t="s">
         <v>415</v>
       </c>
-      <c r="G107" t="s">
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" s="21" t="s">
+        <v>419</v>
+      </c>
+      <c r="B108" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A108" s="22" t="s">
+      <c r="C108" s="9" t="s">
+        <v>417</v>
+      </c>
+      <c r="D108" s="9">
+        <v>1.279401</v>
+      </c>
+      <c r="E108" s="6">
+        <v>103.852964</v>
+      </c>
+      <c r="G108" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" s="21" t="s">
         <v>420</v>
       </c>
-      <c r="B108" t="s">
-        <v>417</v>
-      </c>
-      <c r="C108" s="10" t="s">
-        <v>418</v>
-      </c>
-      <c r="D108" s="10">
-        <v>1.279401</v>
-      </c>
-      <c r="E108" s="7">
-        <v>103.852964</v>
-      </c>
-      <c r="G108" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A109" s="22" t="s">
+      <c r="B109" t="s">
         <v>421</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="C109" s="10" t="s">
+      <c r="D109" s="9">
+        <v>1.2820450000000001</v>
+      </c>
+      <c r="E109" s="6">
+        <v>103.848457</v>
+      </c>
+      <c r="F109" s="12" t="s">
         <v>423</v>
       </c>
-      <c r="D109" s="10">
-        <v>1.2820450000000001</v>
-      </c>
-      <c r="E109" s="7">
-        <v>103.848457</v>
-      </c>
-      <c r="F109" s="13" t="s">
+      <c r="G109" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="G109" s="7" t="s">
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" s="21" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A110" s="22" t="s">
+      <c r="B110" t="s">
         <v>426</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="C110" s="10" t="s">
+      <c r="D110" s="9">
+        <v>1.2844370000000001</v>
+      </c>
+      <c r="E110" s="6">
+        <v>103.843264</v>
+      </c>
+      <c r="F110" s="12" t="s">
         <v>428</v>
       </c>
-      <c r="D110" s="10">
-        <v>1.2844370000000001</v>
-      </c>
-      <c r="E110" s="7">
-        <v>103.843264</v>
-      </c>
-      <c r="F110" s="13" t="s">
+      <c r="G110" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="G110" s="7" t="s">
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="B111" t="s">
         <v>431</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="C111" s="10" t="s">
-        <v>433</v>
-      </c>
-      <c r="D111" s="10">
+      <c r="D111" s="9">
         <v>1.385521</v>
       </c>
-      <c r="E111" s="7">
+      <c r="E111" s="6">
         <v>103.743689</v>
       </c>
       <c r="F111">
         <v>689811</v>
       </c>
-      <c r="G111" s="7" t="s">
+      <c r="G111" s="6" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+      <c r="B112" t="s">
         <v>435</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="C112" s="10" t="s">
-        <v>437</v>
-      </c>
-      <c r="D112" s="10">
+      <c r="D112" s="9">
         <v>1.3803289999999999</v>
       </c>
-      <c r="E112" s="7">
+      <c r="E112" s="6">
         <v>103.745062</v>
       </c>
       <c r="F112">
         <v>688265</v>
       </c>
-      <c r="G112" s="7" t="s">
+      <c r="G112" s="6" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="B113" t="s">
         <v>439</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" s="9" t="s">
         <v>440</v>
       </c>
-      <c r="C113" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="D113" s="10">
+      <c r="D113" s="9">
         <v>1.3786560000000001</v>
       </c>
-      <c r="E113" s="7">
+      <c r="E113" s="6">
         <v>103.748881</v>
       </c>
       <c r="F113">
         <v>688266</v>
       </c>
-      <c r="G113" s="7" t="s">
+      <c r="G113" s="6" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="B114" t="s">
         <v>443</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" s="9" t="s">
         <v>444</v>
       </c>
-      <c r="C114" s="10" t="s">
-        <v>445</v>
-      </c>
-      <c r="D114" s="10">
+      <c r="D114" s="9">
         <v>1.376811</v>
       </c>
-      <c r="E114" s="7">
+      <c r="E114" s="6">
         <v>103.752872</v>
       </c>
       <c r="F114">
         <v>688267</v>
       </c>
-      <c r="G114" s="7" t="s">
+      <c r="G114" s="6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="B115" t="s">
         <v>447</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="C115" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="D115" s="10">
+      <c r="D115" s="9">
         <v>1.3784419999999999</v>
       </c>
-      <c r="E115" s="7">
+      <c r="E115" s="6">
         <v>103.75763600000001</v>
       </c>
       <c r="F115">
         <v>689483</v>
       </c>
-      <c r="G115" s="7" t="s">
+      <c r="G115" s="6" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="B116" t="s">
         <v>451</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" s="9" t="s">
         <v>452</v>
       </c>
-      <c r="C116" s="10" t="s">
-        <v>453</v>
-      </c>
-      <c r="D116" s="10">
+      <c r="D116" s="9">
         <v>1.3781969999999999</v>
       </c>
-      <c r="E116" s="7">
+      <c r="E116" s="6">
         <v>103.76354499999999</v>
       </c>
       <c r="F116">
         <v>678270</v>
       </c>
-      <c r="G116" s="7" t="s">
+      <c r="G116" s="6" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+      <c r="B117" t="s">
         <v>455</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="C117" s="10" t="s">
+      <c r="D117" s="9">
+        <v>1.377291</v>
+      </c>
+      <c r="E117" s="6">
+        <v>103.767376</v>
+      </c>
+      <c r="G117" s="6" t="s">
         <v>457</v>
       </c>
-      <c r="D117" s="10">
-        <v>1.377291</v>
-      </c>
-      <c r="E117" s="7">
-        <v>103.767376</v>
-      </c>
-      <c r="G117" s="7" t="s">
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+      <c r="B118" t="s">
         <v>459</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" s="9" t="s">
         <v>460</v>
       </c>
-      <c r="C118" s="10" t="s">
+      <c r="D118" s="9">
+        <v>1.376261</v>
+      </c>
+      <c r="E118" s="6">
+        <v>103.77131300000001</v>
+      </c>
+      <c r="G118" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="D118" s="10">
-        <v>1.376261</v>
-      </c>
-      <c r="E118" s="7">
-        <v>103.77131300000001</v>
-      </c>
-      <c r="G118" s="7" t="s">
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+      <c r="B119" t="s">
         <v>463</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" s="9" t="s">
         <v>464</v>
       </c>
-      <c r="C119" s="10" t="s">
-        <v>465</v>
-      </c>
-      <c r="D119" s="10">
+      <c r="D119" s="9">
         <v>1.3803909999999999</v>
       </c>
-      <c r="E119" s="7">
+      <c r="E119" s="6">
         <v>103.772622</v>
       </c>
       <c r="F119">
         <v>679939</v>
       </c>
-      <c r="G119" s="7" t="s">
+      <c r="G119" s="6" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+      <c r="B120" t="s">
         <v>467</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" s="9" t="s">
         <v>468</v>
       </c>
-      <c r="C120" s="10" t="s">
-        <v>469</v>
-      </c>
-      <c r="D120" s="10">
+      <c r="D120" s="9">
         <v>1.3847449999999999</v>
       </c>
-      <c r="E120" s="7">
+      <c r="E120" s="6">
         <v>103.77107700000001</v>
       </c>
       <c r="F120">
         <v>679004</v>
       </c>
-      <c r="G120" s="7" t="s">
+      <c r="G120" s="6" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+      <c r="B121" t="s">
         <v>471</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" s="9" t="s">
         <v>472</v>
       </c>
-      <c r="C121" s="10" t="s">
-        <v>473</v>
-      </c>
-      <c r="D121" s="10">
+      <c r="D121" s="9">
         <v>1.387491</v>
       </c>
-      <c r="E121" s="7">
+      <c r="E121" s="6">
         <v>103.77017600000001</v>
       </c>
       <c r="F121">
         <v>679940</v>
       </c>
-      <c r="G121" s="7" t="s">
+      <c r="G121" s="6" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
+      <c r="B122" t="s">
         <v>475</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" s="9" t="s">
         <v>476</v>
       </c>
-      <c r="C122" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="D122" s="10">
+      <c r="D122" s="9">
         <v>1.3868050000000001</v>
       </c>
-      <c r="E122" s="7">
+      <c r="E122" s="6">
         <v>103.764661</v>
       </c>
       <c r="F122">
         <v>679941</v>
       </c>
-      <c r="G122" s="7" t="s">
+      <c r="G122" s="6" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+      <c r="B123" t="s">
         <v>479</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="C123" s="10" t="s">
+      <c r="D123" s="9">
+        <v>1.383211</v>
+      </c>
+      <c r="E123" s="6">
+        <v>103.76216100000001</v>
+      </c>
+      <c r="G123" s="6" t="s">
         <v>481</v>
       </c>
-      <c r="D123" s="10">
-        <v>1.383211</v>
-      </c>
-      <c r="E123" s="7">
-        <v>103.76216100000001</v>
-      </c>
-      <c r="G123" s="7" t="s">
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
+      <c r="B124" t="s">
         <v>483</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>484</v>
-      </c>
-      <c r="C124" t="s">
-        <v>485</v>
       </c>
       <c r="D124">
         <v>1.4047289999999999</v>
@@ -5538,18 +5529,18 @@
         <v>828868</v>
       </c>
       <c r="G124" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
+      <c r="B125" t="s">
         <v>487</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>488</v>
-      </c>
-      <c r="C125" t="s">
-        <v>489</v>
       </c>
       <c r="D125">
         <v>1.3993370000000001</v>
@@ -5561,18 +5552,18 @@
         <v>820198</v>
       </c>
       <c r="G125" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
+      <c r="B126" t="s">
         <v>491</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>492</v>
-      </c>
-      <c r="C126" t="s">
-        <v>493</v>
       </c>
       <c r="D126">
         <v>1.3969780000000001</v>
@@ -5581,18 +5572,18 @@
         <v>103.909177</v>
       </c>
       <c r="G126" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="A127" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
+      <c r="B127" t="s">
         <v>495</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" t="s">
         <v>496</v>
-      </c>
-      <c r="C127" t="s">
-        <v>497</v>
       </c>
       <c r="D127">
         <v>1.393448</v>
@@ -5601,18 +5592,18 @@
         <v>103.91209600000001</v>
       </c>
       <c r="G127" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
+      <c r="B128" t="s">
         <v>499</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" t="s">
         <v>500</v>
-      </c>
-      <c r="C128" t="s">
-        <v>501</v>
       </c>
       <c r="D128">
         <v>1.3946190000000001</v>
@@ -5624,18 +5615,18 @@
         <v>828852</v>
       </c>
       <c r="G128" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
+      <c r="B129" t="s">
         <v>503</v>
       </c>
-      <c r="B129" t="s">
+      <c r="C129" t="s">
         <v>504</v>
-      </c>
-      <c r="C129" t="s">
-        <v>505</v>
       </c>
       <c r="D129">
         <v>1.399338</v>
@@ -5647,18 +5638,18 @@
         <v>828853</v>
       </c>
       <c r="G129" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
+      <c r="B130" t="s">
         <v>507</v>
       </c>
-      <c r="B130" t="s">
+      <c r="C130" t="s">
         <v>508</v>
-      </c>
-      <c r="C130" t="s">
-        <v>509</v>
       </c>
       <c r="D130">
         <v>1.4016120000000001</v>
@@ -5667,18 +5658,18 @@
         <v>103.913605</v>
       </c>
       <c r="G130" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
+      <c r="B131" t="s">
         <v>511</v>
       </c>
-      <c r="B131" t="s">
+      <c r="C131" t="s">
         <v>512</v>
-      </c>
-      <c r="C131" t="s">
-        <v>513</v>
       </c>
       <c r="D131">
         <v>1.4053450000000001</v>
@@ -5690,18 +5681,18 @@
         <v>822612</v>
       </c>
       <c r="G131" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
+      <c r="B132" t="s">
         <v>515</v>
       </c>
-      <c r="B132" t="s">
+      <c r="C132" t="s">
         <v>516</v>
-      </c>
-      <c r="C132" t="s">
-        <v>517</v>
       </c>
       <c r="D132">
         <v>1.391745</v>
@@ -5713,18 +5704,18 @@
         <v>545062</v>
       </c>
       <c r="G132" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
+      <c r="A133" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
+      <c r="B133" t="s">
         <v>519</v>
       </c>
-      <c r="B133" t="s">
+      <c r="C133" t="s">
         <v>520</v>
-      </c>
-      <c r="C133" t="s">
-        <v>521</v>
       </c>
       <c r="D133">
         <v>1.3946190000000001</v>
@@ -5736,18 +5727,18 @@
         <v>540250</v>
       </c>
       <c r="G133" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
+      <c r="A134" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
+      <c r="B134" t="s">
         <v>523</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>524</v>
-      </c>
-      <c r="C134" t="s">
-        <v>525</v>
       </c>
       <c r="D134">
         <v>1.3911009999999999</v>
@@ -5756,18 +5747,18 @@
         <v>103.90622399999999</v>
       </c>
       <c r="G134" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
+      <c r="A135" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
+      <c r="B135" t="s">
         <v>527</v>
       </c>
-      <c r="B135" t="s">
+      <c r="C135" t="s">
         <v>528</v>
-      </c>
-      <c r="C135" t="s">
-        <v>529</v>
       </c>
       <c r="D135">
         <v>1.387883</v>
@@ -5779,18 +5770,18 @@
         <v>545053</v>
       </c>
       <c r="G135" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
+      <c r="B136" t="s">
         <v>531</v>
       </c>
-      <c r="B136" t="s">
+      <c r="C136" t="s">
         <v>532</v>
-      </c>
-      <c r="C136" t="s">
-        <v>533</v>
       </c>
       <c r="D136">
         <v>1.3837219999999999</v>
@@ -5802,18 +5793,18 @@
         <v>545052</v>
       </c>
       <c r="G136" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
+      <c r="A137" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
+      <c r="B137" t="s">
         <v>535</v>
       </c>
-      <c r="B137" t="s">
+      <c r="C137" t="s">
         <v>536</v>
-      </c>
-      <c r="C137" t="s">
-        <v>537</v>
       </c>
       <c r="D137">
         <v>1.3836360000000001</v>
@@ -5822,18 +5813,18 @@
         <v>103.89764099999999</v>
       </c>
       <c r="G137" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
+      <c r="B138" t="s">
         <v>539</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" t="s">
         <v>540</v>
-      </c>
-      <c r="C138" t="s">
-        <v>541</v>
       </c>
       <c r="D138">
         <v>1.397295</v>
@@ -5845,18 +5836,18 @@
         <v>545048</v>
       </c>
       <c r="G138" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7">
+      <c r="A139" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
+      <c r="B139" t="s">
         <v>543</v>
       </c>
-      <c r="B139" t="s">
+      <c r="C139" t="s">
         <v>544</v>
-      </c>
-      <c r="C139" t="s">
-        <v>545</v>
       </c>
       <c r="D139">
         <v>1.397348</v>
@@ -5868,18 +5859,18 @@
         <v>797699</v>
       </c>
       <c r="G139" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7">
+      <c r="A140" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
+      <c r="B140" t="s">
         <v>547</v>
       </c>
-      <c r="B140" t="s">
+      <c r="C140" t="s">
         <v>548</v>
-      </c>
-      <c r="C140" t="s">
-        <v>549</v>
       </c>
       <c r="D140">
         <v>1.391921</v>
@@ -5891,18 +5882,18 @@
         <v>797698</v>
       </c>
       <c r="G140" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7">
+      <c r="A141" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+      <c r="B141" t="s">
         <v>551</v>
       </c>
-      <c r="B141" t="s">
+      <c r="C141" t="s">
         <v>552</v>
-      </c>
-      <c r="C141" t="s">
-        <v>553</v>
       </c>
       <c r="D141">
         <v>1.3921570000000001</v>
@@ -5914,18 +5905,18 @@
         <v>797700</v>
       </c>
       <c r="G141" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7">
+      <c r="A142" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
+      <c r="B142" t="s">
         <v>555</v>
       </c>
-      <c r="B142" t="s">
+      <c r="C142" t="s">
         <v>556</v>
-      </c>
-      <c r="C142" t="s">
-        <v>557</v>
       </c>
       <c r="D142">
         <v>1.3892610000000001</v>
@@ -5937,18 +5928,18 @@
         <v>545050</v>
       </c>
       <c r="G142" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7">
+      <c r="A143" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
+      <c r="B143" t="s">
         <v>559</v>
       </c>
-      <c r="B143" t="s">
+      <c r="C143" t="s">
         <v>560</v>
-      </c>
-      <c r="C143" t="s">
-        <v>561</v>
       </c>
       <c r="D143">
         <v>1.386644</v>
@@ -5960,198 +5951,198 @@
         <v>545049</v>
       </c>
       <c r="G143" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A144" s="17" t="s">
-        <v>565</v>
+        <v>561</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" s="16" t="s">
+        <v>564</v>
       </c>
       <c r="B144" t="s">
-        <v>575</v>
-      </c>
-      <c r="C144" s="10" t="s">
-        <v>453</v>
-      </c>
-      <c r="D144" s="10">
+        <v>574</v>
+      </c>
+      <c r="C144" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="D144" s="9">
         <v>1.3781969999999999</v>
       </c>
-      <c r="E144" s="7">
+      <c r="E144" s="6">
         <v>103.76354499999999</v>
       </c>
       <c r="F144">
         <v>678270</v>
       </c>
-      <c r="G144" s="7" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A145" s="17" t="s">
+      <c r="G144" s="6" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" s="16" t="s">
+        <v>565</v>
+      </c>
+      <c r="B145" t="s">
+        <v>575</v>
+      </c>
+      <c r="D145" s="15">
+        <v>1.3689750000000001</v>
+      </c>
+      <c r="E145" s="6">
+        <v>103.764803</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B146" t="s">
         <v>576</v>
       </c>
-      <c r="D145" s="16">
-        <v>1.3689750000000001</v>
-      </c>
-      <c r="E145" s="7">
-        <v>103.764803</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A146" s="17" t="s">
+      <c r="D146" s="15">
+        <v>1.3624719999999999</v>
+      </c>
+      <c r="E146" s="6">
+        <v>103.76738899999999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B147" t="s">
         <v>577</v>
       </c>
-      <c r="D146" s="16">
-        <v>1.3624719999999999</v>
-      </c>
-      <c r="E146" s="7">
-        <v>103.76738899999999</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A147" s="17" t="s">
+      <c r="D147" s="15">
+        <v>1.3411329999999999</v>
+      </c>
+      <c r="E147" s="6">
+        <v>103.775797</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148" s="16" t="s">
         <v>568</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B148" t="s">
         <v>578</v>
       </c>
-      <c r="D147" s="16">
-        <v>1.3411329999999999</v>
-      </c>
-      <c r="E147" s="7">
-        <v>103.775797</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A148" s="17" t="s">
+      <c r="D148" s="15">
+        <v>1.335628</v>
+      </c>
+      <c r="E148" s="6">
+        <v>103.78398300000001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149" s="16" t="s">
         <v>569</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B149" t="s">
         <v>579</v>
       </c>
-      <c r="D148" s="16">
-        <v>1.335628</v>
-      </c>
-      <c r="E148" s="7">
-        <v>103.78398300000001</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A149" s="17" t="s">
+      <c r="D149" s="15">
+        <v>1.330714</v>
+      </c>
+      <c r="E149" s="6">
+        <v>103.797633</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B150" t="s">
         <v>580</v>
       </c>
-      <c r="D149" s="16">
-        <v>1.330714</v>
-      </c>
-      <c r="E149" s="7">
-        <v>103.797633</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A150" s="17" t="s">
+      <c r="D150" s="15">
+        <v>1.326039</v>
+      </c>
+      <c r="E150" s="6">
+        <v>103.807169</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B151" t="s">
         <v>581</v>
       </c>
-      <c r="D150" s="16">
-        <v>1.326039</v>
-      </c>
-      <c r="E150" s="7">
-        <v>103.807169</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A151" s="17" t="s">
+      <c r="C151" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="D151" s="9">
+        <v>1.3225089999999999</v>
+      </c>
+      <c r="E151" s="6">
+        <v>103.815376</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B152" t="s">
         <v>582</v>
       </c>
-      <c r="C151" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="D151" s="10">
-        <v>1.3225089999999999</v>
-      </c>
-      <c r="E151" s="7">
-        <v>103.815376</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A152" s="17" t="s">
+      <c r="D152" s="15">
+        <v>1.3200689999999999</v>
+      </c>
+      <c r="E152" s="6">
+        <v>103.825997</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" s="16" t="s">
         <v>573</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B153" t="s">
         <v>583</v>
       </c>
-      <c r="D152" s="16">
-        <v>1.3200689999999999</v>
-      </c>
-      <c r="E152" s="7">
-        <v>103.825997</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A153" s="17" t="s">
-        <v>574</v>
-      </c>
-      <c r="B153" t="s">
-        <v>584</v>
-      </c>
-      <c r="C153" s="10" t="s">
-        <v>196</v>
+      <c r="C153" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="D153">
         <v>1.312487</v>
       </c>
-      <c r="E153" s="7">
+      <c r="E153" s="6">
         <v>103.837924</v>
       </c>
       <c r="F153">
         <v>228234</v>
       </c>
       <c r="G153" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A154" s="17" t="s">
-        <v>564</v>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
+      <c r="A154" s="16" t="s">
+        <v>563</v>
       </c>
       <c r="B154" t="s">
+        <v>584</v>
+      </c>
+      <c r="C154" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="D154" s="9">
+        <v>1.3072280000000001</v>
+      </c>
+      <c r="E154" s="6">
+        <v>103.849847</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" s="16" t="s">
+        <v>562</v>
+      </c>
+      <c r="B155" t="s">
         <v>585</v>
       </c>
-      <c r="C154" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="D154" s="10">
-        <v>1.3072280000000001</v>
-      </c>
-      <c r="E154" s="7">
-        <v>103.849847</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A155" s="17" t="s">
-        <v>563</v>
-      </c>
-      <c r="B155" t="s">
-        <v>586</v>
-      </c>
-      <c r="D155" s="16">
+      <c r="D155" s="15">
         <v>1.3037639999999999</v>
       </c>
-      <c r="E155" s="7">
+      <c r="E155" s="6">
         <v>103.852581</v>
       </c>
     </row>
@@ -6168,7 +6159,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6181,7 +6172,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>